<commit_message>
Atualização de versões e dos modelos
</commit_message>
<xml_diff>
--- a/StatisticTests/models/Tables/impact.xlsx
+++ b/StatisticTests/models/Tables/impact.xlsx
@@ -121,13 +121,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>8.127542163203543E-5</v>
+        <v>7.788606327716284E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.1227029553217002E-4</v>
+        <v>1.1227333322968924E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>1.485646760161598E-4</v>
+        <v>1.4529369681869737E-4</v>
       </c>
     </row>
     <row r="4">
@@ -135,13 +135,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>1.2149047112634938E-5</v>
+        <v>9.907462619058397E-6</v>
       </c>
       <c r="C4" t="n">
-        <v>6.174202808432047E-5</v>
+        <v>6.164851215153988E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.234550100371405E-4</v>
+        <v>1.0155627977794528E-4</v>
       </c>
     </row>
     <row r="5">
@@ -149,13 +149,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>3.8971366439164416E-5</v>
+        <v>4.066267089880354E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>9.610430990153552E-5</v>
+        <v>9.63258290780013E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.6517348061829946E-4</v>
+        <v>1.4073969916195432E-4</v>
       </c>
     </row>
     <row r="6">
@@ -163,13 +163,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>1.7177328654530828E-5</v>
+        <v>1.869387293371952E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>7.890795354740179E-5</v>
+        <v>7.902830121400933E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.4699339392146624E-4</v>
+        <v>1.295011353931652E-4</v>
       </c>
     </row>
     <row r="7">
@@ -177,13 +177,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1.8928975523230188E-5</v>
+        <v>2.373439503542935E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>8.057775404251762E-5</v>
+        <v>8.079189053352592E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>1.4797066271360094E-4</v>
+        <v>1.3057129400170965E-4</v>
       </c>
     </row>
     <row r="8">
@@ -191,13 +191,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.3669699234364858E-5</v>
+        <v>1.9125208487619842E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>7.40825164178214E-5</v>
+        <v>7.424212812400549E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>1.4037706581190347E-4</v>
+        <v>1.2258946885169815E-4</v>
       </c>
     </row>
     <row r="9">
@@ -205,13 +205,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.2355814771517058E-5</v>
+        <v>1.9731264210390855E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>7.038946353394904E-5</v>
+        <v>7.056599148624484E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>1.352422328925834E-4</v>
+        <v>1.1634016242442423E-4</v>
       </c>
     </row>
     <row r="10">
@@ -219,13 +219,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.033024436594801E-5</v>
+        <v>1.85267778039415E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>6.577027323233388E-5</v>
+        <v>6.592130203227484E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>1.2875723664545807E-4</v>
+        <v>1.0921448105452198E-4</v>
       </c>
     </row>
     <row r="11">
@@ -233,13 +233,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>8.880647426109942E-6</v>
+        <v>1.7507169858825505E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>6.164758261637729E-5</v>
+        <v>6.179297058571939E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>1.2284226485542217E-4</v>
+        <v>1.0244479312415438E-4</v>
       </c>
     </row>
     <row r="12">
@@ -247,13 +247,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>7.418021567538071E-6</v>
+        <v>1.6237684542212513E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>5.7528333403057836E-5</v>
+        <v>5.766187732111343E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.1678459758430196E-4</v>
+        <v>9.610309374018091E-5</v>
       </c>
     </row>
   </sheetData>
@@ -302,13 +302,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.453309822912089E-4</v>
+        <v>1.4234111911400329E-4</v>
       </c>
       <c r="C3" t="n">
-        <v>1.7433407056613524E-4</v>
+        <v>1.7410737517854685E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.209627237222382E-4</v>
+        <v>2.1177124659676262E-4</v>
       </c>
     </row>
     <row r="4">
@@ -316,13 +316,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>9.163856734172859E-5</v>
+        <v>9.522312194822713E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.415406971710867E-4</v>
+        <v>1.412472388541856E-4</v>
       </c>
       <c r="D4" t="n">
-        <v>1.989532787572923E-4</v>
+        <v>1.969848777966954E-4</v>
       </c>
     </row>
     <row r="5">
@@ -330,13 +330,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.3476238412204092E-4</v>
+        <v>1.3650663073306034E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>1.8413743388977216E-4</v>
+        <v>1.8264925733734033E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>2.466488893610087E-4</v>
+        <v>2.419131455878462E-4</v>
       </c>
     </row>
     <row r="6">
@@ -344,13 +344,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>1.1802583782810878E-4</v>
+        <v>1.2206777110847239E-4</v>
       </c>
       <c r="C6" t="n">
-        <v>1.722354206738748E-4</v>
+        <v>1.7121983881448392E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>2.3563466537674283E-4</v>
+        <v>2.3444985110901046E-4</v>
       </c>
     </row>
     <row r="7">
@@ -358,13 +358,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1.1768813950020775E-4</v>
+        <v>1.2106580584886212E-4</v>
       </c>
       <c r="C7" t="n">
-        <v>1.7173964570331714E-4</v>
+        <v>1.7059524707705733E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>2.3517334550761482E-4</v>
+        <v>2.3131185950273967E-4</v>
       </c>
     </row>
     <row r="8">
@@ -372,13 +372,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.1327810096761111E-4</v>
+        <v>1.1685664954001704E-4</v>
       </c>
       <c r="C8" t="n">
-        <v>1.6722979300180056E-4</v>
+        <v>1.6612517615724673E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>2.289577310893716E-4</v>
+        <v>2.2616193458997375E-4</v>
       </c>
     </row>
     <row r="9">
@@ -386,13 +386,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.1028760029570207E-4</v>
+        <v>1.129705263229843E-4</v>
       </c>
       <c r="C9" t="n">
-        <v>1.6267083321546642E-4</v>
+        <v>1.616111347609355E-4</v>
       </c>
       <c r="D9" t="n">
-        <v>2.215189063084516E-4</v>
+        <v>2.205205149727174E-4</v>
       </c>
     </row>
     <row r="10">
@@ -400,13 +400,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.075403005193386E-4</v>
+        <v>1.0835163047234861E-4</v>
       </c>
       <c r="C10" t="n">
-        <v>1.5849329488988194E-4</v>
+        <v>1.574281033005782E-4</v>
       </c>
       <c r="D10" t="n">
-        <v>2.15547232955986E-4</v>
+        <v>2.1514583265394506E-4</v>
       </c>
     </row>
     <row r="11">
@@ -414,13 +414,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.0467929836291709E-4</v>
+        <v>1.0375552191583413E-4</v>
       </c>
       <c r="C11" t="n">
-        <v>1.541097606603587E-4</v>
+        <v>1.5308354835585544E-4</v>
       </c>
       <c r="D11" t="n">
-        <v>2.096927280660591E-4</v>
+        <v>2.0967349030815037E-4</v>
       </c>
     </row>
     <row r="12">
@@ -428,13 +428,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.0123790825036777E-4</v>
+        <v>9.937337345717014E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.4991857570480625E-4</v>
+        <v>1.4891820576746042E-4</v>
       </c>
       <c r="D12" t="n">
-        <v>2.0456172252419794E-4</v>
+        <v>2.0509512774961585E-4</v>
       </c>
     </row>
   </sheetData>
@@ -483,13 +483,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>8.04326737668289E-5</v>
+        <v>7.091956719175574E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0028219121126138E-4</v>
+        <v>1.0012419555022948E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>1.2165665826753586E-4</v>
+        <v>1.2561428553158117E-4</v>
       </c>
     </row>
     <row r="4">
@@ -497,13 +497,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>9.47935529012298E-6</v>
+        <v>1.792662214545147E-6</v>
       </c>
       <c r="C4" t="n">
-        <v>3.897262116694809E-5</v>
+        <v>3.8852002550604517E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>6.88787148244728E-5</v>
+        <v>6.312900859074564E-5</v>
       </c>
     </row>
     <row r="5">
@@ -511,13 +511,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>3.7019001684423406E-5</v>
+        <v>3.157163141313998E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>7.150260124495715E-5</v>
+        <v>7.01861784836642E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0501510143474317E-4</v>
+        <v>9.909206573470313E-5</v>
       </c>
     </row>
     <row r="6">
@@ -525,13 +525,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>1.790659892782978E-5</v>
+        <v>1.1913185309001396E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>5.530088681648376E-5</v>
+        <v>5.448454658813061E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>9.128372345472706E-5</v>
+        <v>8.434591013592258E-5</v>
       </c>
     </row>
     <row r="7">
@@ -539,13 +539,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1.958609405143751E-5</v>
+        <v>1.5331295270351175E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>5.7581615031383654E-5</v>
+        <v>5.6572869540849805E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>9.56786028304259E-5</v>
+        <v>8.906056491634568E-5</v>
       </c>
     </row>
     <row r="8">
@@ -553,13 +553,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.7041657962240225E-5</v>
+        <v>1.2964943391336118E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>5.431370840482554E-5</v>
+        <v>5.334206251361747E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>9.183019134190893E-5</v>
+        <v>8.50851456592981E-5</v>
       </c>
     </row>
     <row r="9">
@@ -567,13 +567,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.5986678953264073E-5</v>
+        <v>1.2592341862762647E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>5.223985002522828E-5</v>
+        <v>5.1329178474598384E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>8.932427723352535E-5</v>
+        <v>8.370360634499077E-5</v>
       </c>
     </row>
     <row r="10">
@@ -581,13 +581,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.5395400843925534E-5</v>
+        <v>1.3111118162874652E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>5.035146788485119E-5</v>
+        <v>4.9429964331256216E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>8.642874588095385E-5</v>
+        <v>8.20703852014122E-5</v>
       </c>
     </row>
     <row r="11">
@@ -595,13 +595,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.5065582133674216E-5</v>
+        <v>1.3382851885801779E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>4.8302750401299644E-5</v>
+        <v>4.743259322203999E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>8.311587494626838E-5</v>
+        <v>8.04132940392834E-5</v>
       </c>
     </row>
     <row r="12">
@@ -609,13 +609,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.5169469196345825E-5</v>
+        <v>1.3949066333960944E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>4.644757370993685E-5</v>
+        <v>4.559799473529613E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>8.014086012612836E-5</v>
+        <v>7.869241474927907E-5</v>
       </c>
     </row>
   </sheetData>
@@ -664,13 +664,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.5392872026182374E-4</v>
+        <v>1.969098760068898E-4</v>
       </c>
       <c r="C3" t="n">
-        <v>3.10500851404745E-4</v>
+        <v>3.1040080826109673E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>4.431004420034226E-4</v>
+        <v>4.315192800523705E-4</v>
       </c>
     </row>
     <row r="4">
@@ -678,13 +678,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.6446580187679365E-4</v>
+        <v>-1.6759211590305301E-4</v>
       </c>
       <c r="C4" t="n">
-        <v>7.75878507772408E-6</v>
+        <v>7.420303133621358E-6</v>
       </c>
       <c r="D4" t="n">
-        <v>1.656002370494736E-4</v>
+        <v>1.6507023201189986E-4</v>
       </c>
     </row>
     <row r="5">
@@ -692,13 +692,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-5.752340528350125E-5</v>
+        <v>-5.3959280704099406E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>1.298483472875104E-4</v>
+        <v>1.2883429051932044E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>2.9861277010075895E-4</v>
+        <v>2.8510528571845553E-4</v>
       </c>
     </row>
     <row r="6">
@@ -706,13 +706,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.2354545912325246E-4</v>
+        <v>-1.2719508456997654E-4</v>
       </c>
       <c r="C6" t="n">
-        <v>6.217909146701681E-5</v>
+        <v>6.199148906617042E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>2.2791561450225385E-4</v>
+        <v>2.2342113791467525E-4</v>
       </c>
     </row>
     <row r="7">
@@ -720,13 +720,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.1718412671633521E-4</v>
+        <v>-1.1444371498336799E-4</v>
       </c>
       <c r="C7" t="n">
-        <v>7.059784233296086E-5</v>
+        <v>7.028460193259142E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>2.327114749826131E-4</v>
+        <v>2.224994604050093E-4</v>
       </c>
     </row>
     <row r="8">
@@ -734,13 +734,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.1531511970126834E-4</v>
+        <v>-1.1602112608096509E-4</v>
       </c>
       <c r="C8" t="n">
-        <v>6.403731496578666E-5</v>
+        <v>6.372057492355502E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>2.211769740697146E-4</v>
+        <v>2.070026719957699E-4</v>
       </c>
     </row>
     <row r="9">
@@ -748,13 +748,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.1194868607426091E-4</v>
+        <v>-1.156089323024522E-4</v>
       </c>
       <c r="C9" t="n">
-        <v>6.118227740530665E-5</v>
+        <v>6.092031344722925E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>2.122444714083585E-4</v>
+        <v>1.9526273857856314E-4</v>
       </c>
     </row>
     <row r="10">
@@ -762,13 +762,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.0166594349595742E-4</v>
+        <v>-1.0762585291145778E-4</v>
       </c>
       <c r="C10" t="n">
-        <v>6.017310878766818E-5</v>
+        <v>5.983537837627215E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>2.048947555096338E-4</v>
+        <v>1.880242741462638E-4</v>
       </c>
     </row>
     <row r="11">
@@ -776,13 +776,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-9.26556796338858E-5</v>
+        <v>-1.0157002816310476E-4</v>
       </c>
       <c r="C11" t="n">
-        <v>5.8324233116169176E-5</v>
+        <v>5.801942080597748E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>1.973964520598204E-4</v>
+        <v>1.8345924067868203E-4</v>
       </c>
     </row>
     <row r="12">
@@ -790,13 +790,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-8.27586940244238E-5</v>
+        <v>-9.51560195040485E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>5.7093331317128806E-5</v>
+        <v>5.678535102248881E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.9087258468492236E-4</v>
+        <v>1.7974423837349365E-4</v>
       </c>
     </row>
   </sheetData>
@@ -845,13 +845,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>7.317476527639742E-5</v>
+        <v>6.156585308675435E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.4214052889379098E-4</v>
+        <v>1.4249870389588328E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.0620576074308883E-4</v>
+        <v>2.2916338951658227E-4</v>
       </c>
     </row>
     <row r="4">
@@ -859,13 +859,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-4.424592908594365E-5</v>
+        <v>-5.063005796825176E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>5.978589307756733E-5</v>
+        <v>5.987462174207477E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.635886002676142E-4</v>
+        <v>1.8054911335606014E-4</v>
       </c>
     </row>
     <row r="5">
@@ -873,13 +873,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.047142793399986E-5</v>
+        <v>-2.2598096809953933E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>8.974709932354298E-5</v>
+        <v>9.187242548310989E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.982237024866851E-4</v>
+        <v>2.0739160982521365E-4</v>
       </c>
     </row>
     <row r="6">
@@ -887,13 +887,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-2.7045486736932097E-5</v>
+        <v>-3.7711965669774794E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>7.67901996041444E-5</v>
+        <v>7.841866398592984E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.8483588036508693E-4</v>
+        <v>1.985100849150418E-4</v>
       </c>
     </row>
     <row r="7">
@@ -901,13 +901,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-2.9276803040802687E-5</v>
+        <v>-3.715704133176009E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>7.445561906144754E-5</v>
+        <v>7.623138381577491E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>1.821834329058902E-4</v>
+        <v>1.9921456305732884E-4</v>
       </c>
     </row>
     <row r="8">
@@ -915,13 +915,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-2.8923343937799465E-5</v>
+        <v>-3.512065212675169E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>7.322070084641554E-5</v>
+        <v>7.482911173579641E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>1.7825184164944926E-4</v>
+        <v>1.9999305612982234E-4</v>
       </c>
     </row>
     <row r="9">
@@ -929,13 +929,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-2.829680820847869E-5</v>
+        <v>-3.270020690573896E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>7.164885874303842E-5</v>
+        <v>7.321546035986447E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>1.7526960802393326E-4</v>
+        <v>2.003662498252907E-4</v>
       </c>
     </row>
     <row r="10">
@@ -943,13 +943,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.718929728515068E-5</v>
+        <v>-3.2670830090539705E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>7.070019796270538E-5</v>
+        <v>7.218522024336013E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>1.7309883456027665E-4</v>
+        <v>2.011900986651373E-4</v>
       </c>
     </row>
     <row r="11">
@@ -957,13 +957,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.7128308737408555E-5</v>
+        <v>-3.1954274405012885E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>6.961561004269254E-5</v>
+        <v>7.104997308005188E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>1.7085247798550243E-4</v>
+        <v>2.0120640228114231E-4</v>
       </c>
     </row>
     <row r="12">
@@ -971,13 +971,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-2.8590433826446344E-5</v>
+        <v>-3.108729689855737E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>6.859043519444676E-5</v>
+        <v>6.997309380519168E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.6868864964483633E-4</v>
+        <v>1.9780087326843026E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1026,13 +1026,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>6.308811040163756E-5</v>
+        <v>7.535549971350055E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>9.86816578195632E-5</v>
+        <v>9.861534681090082E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.3082706234371157E-4</v>
+        <v>1.333162508321451E-4</v>
       </c>
     </row>
     <row r="4">
@@ -1040,13 +1040,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.1307533313011843E-5</v>
+        <v>-1.7488798038263326E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.8813544646285074E-5</v>
+        <v>1.866169703499179E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>5.109855537129537E-5</v>
+        <v>6.808093575166314E-5</v>
       </c>
     </row>
     <row r="5">
@@ -1054,13 +1054,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.3734202446787305E-5</v>
+        <v>2.145657360367816E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>5.8542924257044464E-5</v>
+        <v>5.810230049015097E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0124638001690407E-4</v>
+        <v>1.1672114879853291E-4</v>
       </c>
     </row>
     <row r="6">
@@ -1068,13 +1068,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-9.561983196049748E-6</v>
+        <v>-2.467571785470922E-7</v>
       </c>
       <c r="C6" t="n">
-        <v>3.738845247288284E-5</v>
+        <v>3.716966295057751E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>7.603057728421764E-5</v>
+        <v>9.241610800456484E-5</v>
       </c>
     </row>
     <row r="7">
@@ -1082,13 +1082,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-4.7200279090676415E-6</v>
+        <v>4.5296057763760864E-6</v>
       </c>
       <c r="C7" t="n">
-        <v>3.970001366434876E-5</v>
+        <v>3.942455132685802E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>7.793627074014246E-5</v>
+        <v>9.888715741288626E-5</v>
       </c>
     </row>
     <row r="8">
@@ -1096,13 +1096,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-7.202036753396402E-6</v>
+        <v>2.4821459851797685E-6</v>
       </c>
       <c r="C8" t="n">
-        <v>3.6299998579507256E-5</v>
+        <v>3.601156468420611E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>7.22310473195308E-5</v>
+        <v>9.297592787337224E-5</v>
       </c>
     </row>
     <row r="9">
@@ -1110,13 +1110,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-6.77804219226432E-6</v>
+        <v>2.228919309847089E-6</v>
       </c>
       <c r="C9" t="n">
-        <v>3.470849950571527E-5</v>
+        <v>3.4441502529932155E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>7.019779339342845E-5</v>
+        <v>9.035211712052628E-5</v>
       </c>
     </row>
     <row r="10">
@@ -1124,13 +1124,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-6.60856785455131E-6</v>
+        <v>2.01364424962227E-6</v>
       </c>
       <c r="C10" t="n">
-        <v>3.329991514174805E-5</v>
+        <v>3.30062220558337E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>6.870238764766343E-5</v>
+        <v>8.734314858580059E-5</v>
       </c>
     </row>
     <row r="11">
@@ -1138,13 +1138,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-6.408684984549526E-6</v>
+        <v>1.5057095810933392E-6</v>
       </c>
       <c r="C11" t="n">
-        <v>3.180427212943294E-5</v>
+        <v>3.1523060502715715E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>6.720045629865365E-5</v>
+        <v>8.427867423922235E-5</v>
       </c>
     </row>
     <row r="12">
@@ -1152,13 +1152,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-6.1369624637892625E-6</v>
+        <v>7.834444530083933E-7</v>
       </c>
       <c r="C12" t="n">
-        <v>3.0468582851718875E-5</v>
+        <v>3.0188605535160076E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>6.593042502625848E-5</v>
+        <v>8.161693190649118E-5</v>
       </c>
     </row>
   </sheetData>
@@ -1207,13 +1207,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>4.151445422968892E-5</v>
+        <v>3.838692521586176E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>9.70239438198642E-5</v>
+        <v>9.678035335468398E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.7717911195206496E-4</v>
+        <v>1.525415025179542E-4</v>
       </c>
     </row>
     <row r="4">
@@ -1221,13 +1221,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-9.216308392727704E-5</v>
+        <v>-8.31819394785396E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.2433347837424927E-5</v>
+        <v>-1.282309170464293E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>8.710536633609046E-5</v>
+        <v>6.659445156659765E-5</v>
       </c>
     </row>
     <row r="5">
@@ -1235,13 +1235,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-4.843531317465475E-5</v>
+        <v>-4.0306215027923415E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>2.6639111248295207E-5</v>
+        <v>2.5242487551298982E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.2430303449481033E-4</v>
+        <v>1.0782068020118904E-4</v>
       </c>
     </row>
     <row r="6">
@@ -1249,13 +1249,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-6.745153398298993E-5</v>
+        <v>-5.584641451055214E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>9.9153366042898E-6</v>
+        <v>9.465957493670027E-6</v>
       </c>
       <c r="D6" t="n">
-        <v>1.0312189067651482E-4</v>
+        <v>8.785510861463078E-5</v>
       </c>
     </row>
     <row r="7">
@@ -1263,13 +1263,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-6.967740019934962E-5</v>
+        <v>-5.791281469853503E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>7.402932481513147E-6</v>
+        <v>6.890637466857658E-6</v>
       </c>
       <c r="D7" t="n">
-        <v>9.894229803094948E-5</v>
+        <v>8.339609803451514E-5</v>
       </c>
     </row>
     <row r="8">
@@ -1277,13 +1277,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-6.846698177582185E-5</v>
+        <v>-5.211914619890629E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>7.530482002109847E-6</v>
+        <v>7.044785077397334E-6</v>
       </c>
       <c r="D8" t="n">
-        <v>9.411383222570836E-5</v>
+        <v>7.903685186175814E-5</v>
       </c>
     </row>
     <row r="9">
@@ -1291,13 +1291,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-6.906473042258998E-5</v>
+        <v>-5.104715467030493E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>6.389871558195871E-6</v>
+        <v>5.9422106199520025E-6</v>
       </c>
       <c r="D9" t="n">
-        <v>8.861920750402718E-5</v>
+        <v>7.402615438427571E-5</v>
       </c>
     </row>
     <row r="10">
@@ -1305,13 +1305,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-6.880051551787347E-5</v>
+        <v>-4.825407256183064E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>6.190557528203435E-6</v>
+        <v>5.719284539600355E-6</v>
       </c>
       <c r="D10" t="n">
-        <v>8.449262416547395E-5</v>
+        <v>7.015946324139695E-5</v>
       </c>
     </row>
     <row r="11">
@@ -1319,13 +1319,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-6.854049253629647E-5</v>
+        <v>-4.698767255949897E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>5.700735412580499E-6</v>
+        <v>5.2554716778030546E-6</v>
       </c>
       <c r="D11" t="n">
-        <v>8.118054255517268E-5</v>
+        <v>6.730848621077288E-5</v>
       </c>
     </row>
     <row r="12">
@@ -1333,13 +1333,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-6.742196023452228E-5</v>
+        <v>-4.703323605674094E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>5.255074903995163E-6</v>
+        <v>4.8286052348918824E-6</v>
       </c>
       <c r="D12" t="n">
-        <v>7.918062185202178E-5</v>
+        <v>6.469626712373302E-5</v>
       </c>
     </row>
   </sheetData>
@@ -1388,13 +1388,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.4621171032310802E-4</v>
+        <v>1.335307136246534E-4</v>
       </c>
       <c r="C3" t="n">
-        <v>2.134536363816292E-4</v>
+        <v>2.1421058772919037E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>3.0540428795126917E-4</v>
+        <v>2.844585185242225E-4</v>
       </c>
     </row>
     <row r="4">
@@ -1402,13 +1402,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>2.9740852026388875E-5</v>
+        <v>2.289553886926821E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.137116110658993E-4</v>
+        <v>1.1417334721353804E-4</v>
       </c>
       <c r="D4" t="n">
-        <v>2.1962064476191876E-4</v>
+        <v>2.1888979214301562E-4</v>
       </c>
     </row>
     <row r="5">
@@ -1416,13 +1416,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0411908623920834E-4</v>
+        <v>9.125734908659531E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>1.957972927939293E-4</v>
+        <v>1.980479211853999E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>3.151706179798362E-4</v>
+        <v>3.058176986274442E-4</v>
       </c>
     </row>
     <row r="6">
@@ -1430,13 +1430,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>6.39261399457941E-5</v>
+        <v>5.238699255762715E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.595815470051955E-4</v>
+        <v>1.6154929623911528E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>2.7154687747741436E-4</v>
+        <v>2.741024439708347E-4</v>
       </c>
     </row>
     <row r="7">
@@ -1444,13 +1444,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>6.907386481545186E-5</v>
+        <v>5.6024522250209954E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.629813657195134E-4</v>
+        <v>1.653221013189827E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>2.7427277146903584E-4</v>
+        <v>2.744419918628091E-4</v>
       </c>
     </row>
     <row r="8">
@@ -1458,13 +1458,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>6.364547110116641E-5</v>
+        <v>4.751849075254111E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.5410667714580475E-4</v>
+        <v>1.5626373036631993E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>2.58803977885537E-4</v>
+        <v>2.662794804141646E-4</v>
       </c>
     </row>
     <row r="9">
@@ -1472,13 +1472,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>5.9941987834399174E-5</v>
+        <v>4.253126594277566E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>1.4876807370330195E-4</v>
+        <v>1.5097011487039203E-4</v>
       </c>
       <c r="D9" t="n">
-        <v>2.520889584974489E-4</v>
+        <v>2.649044294095296E-4</v>
       </c>
     </row>
     <row r="10">
@@ -1486,13 +1486,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>5.804752214394907E-5</v>
+        <v>3.71850484046345E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.4357119232288594E-4</v>
+        <v>1.4563419410385648E-4</v>
       </c>
       <c r="D10" t="n">
-        <v>2.442423164472861E-4</v>
+        <v>2.609988641447206E-4</v>
       </c>
     </row>
     <row r="11">
@@ -1500,13 +1500,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>5.954364696086006E-5</v>
+        <v>3.3764248122052625E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.3835595051650532E-4</v>
+        <v>1.4036986394629382E-4</v>
       </c>
       <c r="D11" t="n">
-        <v>2.375719884697875E-4</v>
+        <v>2.5523590006742763E-4</v>
       </c>
     </row>
     <row r="12">
@@ -1514,13 +1514,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>5.953184176930751E-5</v>
+        <v>3.194649872422631E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.3344811636605065E-4</v>
+        <v>1.3539043966379825E-4</v>
       </c>
       <c r="D12" t="n">
-        <v>2.3151931186218022E-4</v>
+        <v>2.49681084726227E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1569,13 +1569,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.0241189344881773E-4</v>
+        <v>1.1137362039218465E-4</v>
       </c>
       <c r="C3" t="n">
-        <v>1.5431540070566757E-4</v>
+        <v>1.5449860641343461E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>1.860890312790138E-4</v>
+        <v>1.8786138045485154E-4</v>
       </c>
     </row>
     <row r="4">
@@ -1583,13 +1583,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>4.2513279903363356E-5</v>
+        <v>4.671565685417173E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>9.669364750886614E-5</v>
+        <v>9.66822093617025E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.4728284426571814E-4</v>
+        <v>1.430004876476057E-4</v>
       </c>
     </row>
     <row r="5">
@@ -1597,13 +1597,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>9.264900178083621E-5</v>
+        <v>1.0079001276719632E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>1.5598829461541507E-4</v>
+        <v>1.566536826326961E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>2.0801004595555466E-4</v>
+        <v>2.1162633016370063E-4</v>
       </c>
     </row>
     <row r="6">
@@ -1611,13 +1611,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>6.611677953850181E-5</v>
+        <v>7.551188988151971E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.3418188225821387E-4</v>
+        <v>1.347013308362997E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>1.9542055602577997E-4</v>
+        <v>1.9694698732431023E-4</v>
       </c>
     </row>
     <row r="7">
@@ -1625,13 +1625,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>7.412595011311228E-5</v>
+        <v>8.249116413677101E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.424778974343251E-4</v>
+        <v>1.4313213403187625E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>2.0483336268171885E-4</v>
+        <v>2.083397808266039E-4</v>
       </c>
     </row>
     <row r="8">
@@ -1639,13 +1639,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>6.77566850635228E-5</v>
+        <v>7.571999936887875E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.354123065013963E-4</v>
+        <v>1.3599317866687944E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>1.9980876319274985E-4</v>
+        <v>2.0283924506731474E-4</v>
       </c>
     </row>
     <row r="9">
@@ -1653,13 +1653,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>6.715370100723952E-5</v>
+        <v>7.379342181082862E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>1.3317247160712806E-4</v>
+        <v>1.3377291955823535E-4</v>
       </c>
       <c r="D9" t="n">
-        <v>1.9744882776160695E-4</v>
+        <v>2.0071618873763677E-4</v>
       </c>
     </row>
     <row r="10">
@@ -1667,13 +1667,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>6.467087913014045E-5</v>
+        <v>6.942584441576926E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.2873768153894602E-4</v>
+        <v>1.292942323036604E-4</v>
       </c>
       <c r="D10" t="n">
-        <v>1.929597481849818E-4</v>
+        <v>1.9578611562174242E-4</v>
       </c>
     </row>
     <row r="11">
@@ -1681,13 +1681,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>6.299625695268419E-5</v>
+        <v>6.616755565218087E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.249166993752008E-4</v>
+        <v>1.254611136238122E-4</v>
       </c>
       <c r="D11" t="n">
-        <v>1.8877165668538712E-4</v>
+        <v>1.8882980663187358E-4</v>
       </c>
     </row>
     <row r="12">
@@ -1695,13 +1695,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>6.102336421854065E-5</v>
+        <v>6.259302901195082E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.2085633500717312E-4</v>
+        <v>1.2137822540814068E-4</v>
       </c>
       <c r="D12" t="n">
-        <v>1.8440228087105722E-4</v>
+        <v>1.818780111076027E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1750,13 +1750,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>3.320518937912626E-5</v>
+        <v>3.489487169049455E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>4.894505782907252E-5</v>
+        <v>4.883943272570913E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>6.441535714577794E-5</v>
+        <v>6.981910487149082E-5</v>
       </c>
     </row>
     <row r="4">
@@ -1764,13 +1764,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.8012056835210142E-5</v>
+        <v>-1.8904128028199486E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.5929569099443934E-6</v>
+        <v>1.489106480457413E-6</v>
       </c>
       <c r="D4" t="n">
-        <v>2.141416853691208E-5</v>
+        <v>3.682751197053154E-5</v>
       </c>
     </row>
     <row r="5">
@@ -1778,13 +1778,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>4.6908855884769076E-7</v>
+        <v>1.1473513753769705E-6</v>
       </c>
       <c r="C5" t="n">
-        <v>2.405739146210201E-5</v>
+        <v>2.3450990313058582E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>4.858620863963328E-5</v>
+        <v>5.7890060207493196E-5</v>
       </c>
     </row>
     <row r="6">
@@ -1792,13 +1792,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.305658034185083E-5</v>
+        <v>-1.2373878199038512E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0004390594879177E-5</v>
+        <v>9.720877136062259E-6</v>
       </c>
       <c r="D6" t="n">
-        <v>3.4248652853317096E-5</v>
+        <v>4.680769206206456E-5</v>
       </c>
     </row>
     <row r="7">
@@ -1806,13 +1806,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.1346752049844814E-5</v>
+        <v>-1.1509070506952588E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.167818945463498E-5</v>
+        <v>1.134680468473094E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>3.6117821179702335E-5</v>
+        <v>4.7780265277822834E-5</v>
       </c>
     </row>
     <row r="8">
@@ -1820,13 +1820,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.2877882442551987E-5</v>
+        <v>-1.2956950294621884E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>9.32896464738799E-6</v>
+        <v>9.02855656706701E-6</v>
       </c>
       <c r="D8" t="n">
-        <v>3.2835171203162486E-5</v>
+        <v>4.3718334317359946E-5</v>
       </c>
     </row>
     <row r="9">
@@ -1834,13 +1834,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.3129208369276742E-5</v>
+        <v>-1.3169256736164048E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>8.606912306965851E-6</v>
+        <v>8.321261606812771E-6</v>
       </c>
       <c r="D9" t="n">
-        <v>3.1830954885280715E-5</v>
+        <v>4.1771352586950715E-5</v>
       </c>
     </row>
     <row r="10">
@@ -1848,13 +1848,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.3131105308948926E-5</v>
+        <v>-1.2929271046744237E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>7.838676322527244E-6</v>
+        <v>7.540860428944782E-6</v>
       </c>
       <c r="D10" t="n">
-        <v>3.05816706528948E-5</v>
+        <v>3.9092386977104736E-5</v>
       </c>
     </row>
     <row r="11">
@@ -1862,13 +1862,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.3227860516710538E-5</v>
+        <v>-1.277442495983109E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>7.1292293341027715E-6</v>
+        <v>6.8449970226986405E-6</v>
       </c>
       <c r="D11" t="n">
-        <v>2.9201944585517426E-5</v>
+        <v>3.678654261968376E-5</v>
       </c>
     </row>
     <row r="12">
@@ -1876,13 +1876,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.3214056394812091E-5</v>
+        <v>-1.3127693339336812E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>6.470774398522533E-6</v>
+        <v>6.191210801842718E-6</v>
       </c>
       <c r="D12" t="n">
-        <v>2.777499678637113E-5</v>
+        <v>3.4456108138368896E-5</v>
       </c>
     </row>
   </sheetData>
@@ -1931,13 +1931,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>5.486397257023084E-5</v>
+        <v>5.269054748315756E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>6.947308114268989E-5</v>
+        <v>6.952223378832964E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>8.097080595089515E-5</v>
+        <v>8.012816312414841E-5</v>
       </c>
     </row>
     <row r="4">
@@ -1945,13 +1945,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>2.1329553223377982E-5</v>
+        <v>2.0409756307212845E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>3.902316928963753E-5</v>
+        <v>3.9065230223776586E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>5.802694101273613E-5</v>
+        <v>5.363519431852723E-5</v>
       </c>
     </row>
     <row r="5">
@@ -1959,13 +1959,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>3.545966781599798E-5</v>
+        <v>3.379424696262023E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>5.285272781809165E-5</v>
+        <v>5.3163984385203124E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>7.287582950465085E-5</v>
+        <v>6.944679175742462E-5</v>
       </c>
     </row>
     <row r="6">
@@ -1973,13 +1973,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>2.6745802574830906E-5</v>
+        <v>2.5488092997502298E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>4.623127667668903E-5</v>
+        <v>4.645994305067936E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>6.716754416382158E-5</v>
+        <v>6.233514861660944E-5</v>
       </c>
     </row>
     <row r="7">
@@ -1987,13 +1987,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>2.5521234761554606E-5</v>
+        <v>2.5273298902273348E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>4.565247008251243E-5</v>
+        <v>4.594788002151691E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>6.585256837174998E-5</v>
+        <v>6.135032985259328E-5</v>
       </c>
     </row>
     <row r="8">
@@ -2001,13 +2001,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>2.227291907420407E-5</v>
+        <v>2.348241034069262E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>4.331316511198585E-5</v>
+        <v>4.354633651957676E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>6.306677812333764E-5</v>
+        <v>5.837684674111875E-5</v>
       </c>
     </row>
     <row r="9">
@@ -2015,13 +2015,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.989057097480423E-5</v>
+        <v>2.196590053049339E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>4.1297924538293E-5</v>
+        <v>4.153565681913716E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>6.044898363972568E-5</v>
+        <v>5.639685531721535E-5</v>
       </c>
     </row>
     <row r="10">
@@ -2029,13 +2029,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.842724585160211E-5</v>
+        <v>2.001190627514488E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>3.930171472199017E-5</v>
+        <v>3.951683236068289E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>5.7744793715934653E-5</v>
+        <v>5.4412698163066124E-5</v>
       </c>
     </row>
     <row r="11">
@@ -2043,13 +2043,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.70981847000537E-5</v>
+        <v>1.809150982015601E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>3.7402202111789624E-5</v>
+        <v>3.7605222186242396E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>5.5138648254073996E-5</v>
+        <v>5.247148935653469E-5</v>
       </c>
     </row>
     <row r="12">
@@ -2057,13 +2057,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.587723391600665E-5</v>
+        <v>1.6307322147875455E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>3.55751986889411E-5</v>
+        <v>3.576521158314071E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>5.262436083711528E-5</v>
+        <v>5.0857186905554935E-5</v>
       </c>
     </row>
   </sheetData>
@@ -2112,13 +2112,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>5.170805719488258E-5</v>
+        <v>5.63424467209158E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.315878765031963E-4</v>
+        <v>1.3126379639707031E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.4507657163409476E-4</v>
+        <v>2.4864761166944356E-4</v>
       </c>
     </row>
     <row r="4">
@@ -2126,13 +2126,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.0455498370986102E-4</v>
+        <v>-1.073650809015569E-4</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.5072139802222203E-6</v>
+        <v>-3.941707487155559E-6</v>
       </c>
       <c r="D4" t="n">
-        <v>1.2256482293960175E-4</v>
+        <v>1.2862408141500048E-4</v>
       </c>
     </row>
     <row r="5">
@@ -2140,13 +2140,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-5.503434191807599E-5</v>
+        <v>-6.694295579916548E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>3.802751731844853E-5</v>
+        <v>3.606743655753299E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.5417217685791736E-4</v>
+        <v>1.5779282512212064E-4</v>
       </c>
     </row>
     <row r="6">
@@ -2154,13 +2154,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-7.311414050572006E-5</v>
+        <v>-8.353218410716925E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.9311561522531366E-5</v>
+        <v>1.873630681574646E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.3676041967174097E-4</v>
+        <v>1.4029671056178664E-4</v>
       </c>
     </row>
     <row r="7">
@@ -2168,13 +2168,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-7.410450207298714E-5</v>
+        <v>-8.93664786589838E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.559316563178556E-5</v>
+        <v>1.5003014982292908E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>1.321876224219565E-4</v>
+        <v>1.3472066024396062E-4</v>
       </c>
     </row>
     <row r="8">
@@ -2182,13 +2182,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-6.976548535044009E-5</v>
+        <v>-8.320937175227101E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.5867287609570392E-5</v>
+        <v>1.530016811253724E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>1.295764593819518E-4</v>
+        <v>1.3337341997235756E-4</v>
       </c>
     </row>
     <row r="9">
@@ -2196,13 +2196,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-6.432783701716231E-5</v>
+        <v>-8.239276748975726E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>1.464376585886997E-5</v>
+        <v>1.4125470081844684E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>1.2479017943805058E-4</v>
+        <v>1.3059036585160366E-4</v>
       </c>
     </row>
     <row r="10">
@@ -2210,13 +2210,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-6.14451807816342E-5</v>
+        <v>-7.994794492147367E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.4501911216762944E-5</v>
+        <v>1.3951378422584053E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>1.2166603673036067E-4</v>
+        <v>1.2977542033775651E-4</v>
       </c>
     </row>
     <row r="11">
@@ -2224,13 +2224,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-5.9175218025000873E-5</v>
+        <v>-7.82788502438476E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.4026861521905276E-5</v>
+        <v>1.35057719453106E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>1.2095503198988592E-4</v>
+        <v>1.2481534878488207E-4</v>
       </c>
     </row>
     <row r="12">
@@ -2238,13 +2238,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-5.886339160016485E-5</v>
+        <v>-7.97979504993474E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.3591772290421806E-5</v>
+        <v>1.3092230423868499E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.2042670228778161E-4</v>
+        <v>1.1901522500840828E-4</v>
       </c>
     </row>
   </sheetData>
@@ -2293,13 +2293,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>9.833452075703775E-6</v>
+        <v>9.758594159660214E-6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.5612679365466378E-5</v>
+        <v>1.561677879826541E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>2.048523260398118E-5</v>
+        <v>2.249558898358798E-5</v>
       </c>
     </row>
     <row r="4">
@@ -2307,13 +2307,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-8.678930067678496E-7</v>
+        <v>-2.535009203447866E-6</v>
       </c>
       <c r="C4" t="n">
-        <v>6.963228752951212E-6</v>
+        <v>6.952768369448205E-6</v>
       </c>
       <c r="D4" t="n">
-        <v>1.3805216938508597E-5</v>
+        <v>1.4720110032071848E-5</v>
       </c>
     </row>
     <row r="5">
@@ -2321,13 +2321,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>3.3623117842837297E-6</v>
+        <v>1.920307593022782E-6</v>
       </c>
       <c r="C5" t="n">
-        <v>1.2666588753599818E-5</v>
+        <v>1.2643282893722446E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>2.070286302371016E-5</v>
+        <v>2.1580758607290077E-5</v>
       </c>
     </row>
     <row r="6">
@@ -2335,13 +2335,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>2.592398872075332E-7</v>
+        <v>-1.2844206807816312E-6</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0136037498668874E-5</v>
+        <v>1.0135991637107659E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.8460445069762677E-5</v>
+        <v>1.9335392193226395E-5</v>
       </c>
     </row>
     <row r="7">
@@ -2349,13 +2349,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>3.0806357866602045E-7</v>
+        <v>-9.828743952145076E-7</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0741323437395615E-5</v>
+        <v>1.0725411401855623E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>1.987720155151196E-5</v>
+        <v>1.9996429326080102E-5</v>
       </c>
     </row>
     <row r="8">
@@ -2363,13 +2363,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.3605737804285407E-7</v>
+        <v>-1.2961431786575484E-6</v>
       </c>
       <c r="C8" t="n">
-        <v>1.0124317472856489E-5</v>
+        <v>1.011064874440811E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>1.9143455720080988E-5</v>
+        <v>1.89165930447901E-5</v>
       </c>
     </row>
     <row r="9">
@@ -2377,13 +2377,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-5.802754451496568E-7</v>
+        <v>-1.35527628919838E-6</v>
       </c>
       <c r="C9" t="n">
-        <v>9.858897836952942E-6</v>
+        <v>9.844934414624075E-6</v>
       </c>
       <c r="D9" t="n">
-        <v>1.8909219606887686E-5</v>
+        <v>1.822110769462304E-5</v>
       </c>
     </row>
     <row r="10">
@@ -2391,13 +2391,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-6.450016176887404E-7</v>
+        <v>-1.3742373114696646E-6</v>
       </c>
       <c r="C10" t="n">
-        <v>9.508324222821874E-6</v>
+        <v>9.492663168732812E-6</v>
       </c>
       <c r="D10" t="n">
-        <v>1.8413635181050587E-5</v>
+        <v>1.7380685351820214E-5</v>
       </c>
     </row>
     <row r="11">
@@ -2405,13 +2405,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-8.461644273826219E-7</v>
+        <v>-1.2291635700988022E-6</v>
       </c>
       <c r="C11" t="n">
-        <v>9.174436923549955E-6</v>
+        <v>9.159550941514867E-6</v>
       </c>
       <c r="D11" t="n">
-        <v>1.7962363853190428E-5</v>
+        <v>1.6826793854481613E-5</v>
       </c>
     </row>
     <row r="12">
@@ -2419,13 +2419,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.2024873228805933E-6</v>
+        <v>-1.025752771203109E-6</v>
       </c>
       <c r="C12" t="n">
-        <v>8.8486641311474E-6</v>
+        <v>8.833473931980752E-6</v>
       </c>
       <c r="D12" t="n">
-        <v>1.744640101020555E-5</v>
+        <v>1.6723043077294172E-5</v>
       </c>
     </row>
   </sheetData>
@@ -2474,13 +2474,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>-7.475508347364106E-6</v>
+        <v>-1.5851425708668273E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>2.620424033733634E-5</v>
+        <v>2.62416236558564E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>6.562905723169256E-5</v>
+        <v>5.8210015966298155E-5</v>
       </c>
     </row>
     <row r="4">
@@ -2488,13 +2488,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-8.573489067280301E-5</v>
+        <v>-9.0275467436097E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.2339558690688076E-5</v>
+        <v>-3.239677056370197E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.9770682605675982E-5</v>
+        <v>1.0967562278109024E-5</v>
       </c>
     </row>
     <row r="5">
@@ -2502,13 +2502,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-6.803701266726261E-5</v>
+        <v>-6.93738690568466E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>-7.856342434096716E-6</v>
+        <v>-7.762046962751636E-6</v>
       </c>
       <c r="D5" t="n">
-        <v>5.1717425155952476E-5</v>
+        <v>4.415275828684073E-5</v>
       </c>
     </row>
     <row r="6">
@@ -2516,13 +2516,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-8.485861727857337E-5</v>
+        <v>-8.791166913437717E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.5150034208418485E-5</v>
+        <v>-2.4886187860625285E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>3.904254469969536E-5</v>
+        <v>2.4824604907010056E-5</v>
       </c>
     </row>
     <row r="7">
@@ -2530,13 +2530,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-8.560149218739061E-5</v>
+        <v>-8.56953704957714E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.3867565410480094E-5</v>
+        <v>-2.353551924099664E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>3.967806406491182E-5</v>
+        <v>2.827269529738472E-5</v>
       </c>
     </row>
     <row r="8">
@@ -2544,13 +2544,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.652778962711943E-5</v>
+        <v>-8.543000172188495E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.5872169276371914E-5</v>
+        <v>-2.5571396824989053E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>3.744563952274222E-5</v>
+        <v>2.4460075765390306E-5</v>
       </c>
     </row>
     <row r="9">
@@ -2558,13 +2558,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-8.626179394413151E-5</v>
+        <v>-8.333013909066266E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>-2.62020239419063E-5</v>
+        <v>-2.59036917145582E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>3.72516418524513E-5</v>
+        <v>2.384227523147164E-5</v>
       </c>
     </row>
     <row r="10">
@@ -2572,13 +2572,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-8.564492526606424E-5</v>
+        <v>-8.105853336010979E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.6300126661176765E-5</v>
+        <v>-2.6042816682326928E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>3.605901072907995E-5</v>
+        <v>2.2993964099507694E-5</v>
       </c>
     </row>
     <row r="11">
@@ -2586,13 +2586,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-8.518246531987057E-5</v>
+        <v>-7.949995843690645E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.6456837420427194E-5</v>
+        <v>-2.6209378306993627E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>3.476119371541974E-5</v>
+        <v>2.2265258954316328E-5</v>
       </c>
     </row>
     <row r="12">
@@ -2600,13 +2600,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-8.470493175334986E-5</v>
+        <v>-7.796808846250977E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.6524465843140927E-5</v>
+        <v>-2.629121594501653E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>3.461248842392279E-5</v>
+        <v>2.165438549270456E-5</v>
       </c>
     </row>
   </sheetData>
@@ -2655,13 +2655,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>6.27931511119734E-5</v>
+        <v>8.735369985747219E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.947906671516495E-4</v>
+        <v>1.9511602990673083E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>3.368343741432558E-4</v>
+        <v>2.9138353750147067E-4</v>
       </c>
     </row>
     <row r="4">
@@ -2669,13 +2669,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-5.391154901221762E-5</v>
+        <v>-6.769407593302612E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0643104480710278E-4</v>
+        <v>1.0617573158201675E-4</v>
       </c>
       <c r="D4" t="n">
-        <v>2.8010232972015744E-4</v>
+        <v>2.798662649768939E-4</v>
       </c>
     </row>
     <row r="5">
@@ -2683,13 +2683,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.1291989764794062E-5</v>
+        <v>-7.121590034908226E-7</v>
       </c>
       <c r="C5" t="n">
-        <v>1.7762203586004478E-4</v>
+        <v>1.7864564318151508E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>3.634056201703724E-4</v>
+        <v>3.6252691695435116E-4</v>
       </c>
     </row>
     <row r="6">
@@ -2697,13 +2697,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-2.1740226301537732E-5</v>
+        <v>-3.6675062116670996E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.4785226155858053E-4</v>
+        <v>1.4867729185341546E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>3.2789697575334297E-4</v>
+        <v>3.2602884925528113E-4</v>
       </c>
     </row>
     <row r="7">
@@ -2711,13 +2711,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-2.8657839287202047E-5</v>
+        <v>-3.6260989054248246E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.41542583373333E-4</v>
+        <v>1.4231967605716068E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>3.1184236296012317E-4</v>
+        <v>3.13895613781596E-4</v>
       </c>
     </row>
     <row r="8">
@@ -2725,13 +2725,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.304913271921782E-5</v>
+        <v>-3.8383307532960105E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.3254033683649536E-4</v>
+        <v>1.3329508253946126E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>2.913958404097323E-4</v>
+        <v>2.942746275517486E-4</v>
       </c>
     </row>
     <row r="9">
@@ -2739,13 +2739,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-3.8256996242202944E-5</v>
+        <v>-4.1487674686389105E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>1.230276668008588E-4</v>
+        <v>1.237562814258342E-4</v>
       </c>
       <c r="D9" t="n">
-        <v>2.739120847660929E-4</v>
+        <v>2.7738348945265394E-4</v>
       </c>
     </row>
     <row r="10">
@@ -2753,13 +2753,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-4.1347164068275705E-5</v>
+        <v>-4.1871326422875945E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.1558773560721863E-4</v>
+        <v>1.1624825461904845E-4</v>
       </c>
       <c r="D10" t="n">
-        <v>2.599913195079813E-4</v>
+        <v>2.615467945811246E-4</v>
       </c>
     </row>
     <row r="11">
@@ -2767,13 +2767,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-4.469597892882778E-5</v>
+        <v>-4.430284656436626E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0781467529164133E-4</v>
+        <v>1.0844502477399524E-4</v>
       </c>
       <c r="D11" t="n">
-        <v>2.464736428926952E-4</v>
+        <v>2.473140329074424E-4</v>
       </c>
     </row>
     <row r="12">
@@ -2781,13 +2781,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-4.780578705608131E-5</v>
+        <v>-4.672290288110072E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0060541629710394E-4</v>
+        <v>1.0120122210850753E-4</v>
       </c>
       <c r="D12" t="n">
-        <v>2.3525468711749672E-4</v>
+        <v>2.3686679356430535E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor sector mapping and improve statistical modeling scripts
</commit_message>
<xml_diff>
--- a/StatisticTests/models/Tables/impact.xlsx
+++ b/StatisticTests/models/Tables/impact.xlsx
@@ -21,12 +21,13 @@
     <sheet name="Telecomunicações" r:id="rId15" sheetId="13"/>
     <sheet name="Transporte" r:id="rId16" sheetId="14"/>
     <sheet name="Utilidade Pública" r:id="rId17" sheetId="15"/>
+    <sheet name="market" r:id="rId18" sheetId="16"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="4">
   <si>
     <t>Days</t>
   </si>
@@ -121,13 +122,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>7.788606327716284E-5</v>
+        <v>6.362379528723003E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.1227333322968924E-4</v>
+        <v>1.0510429289085613E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4529369681869737E-4</v>
+        <v>1.5283459676282733E-4</v>
       </c>
     </row>
     <row r="4">
@@ -135,13 +136,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>9.907462619058397E-6</v>
+        <v>2.839106879092363E-6</v>
       </c>
       <c r="C4" t="n">
-        <v>6.164851215153988E-5</v>
+        <v>5.8251442283294314E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0155627977794528E-4</v>
+        <v>1.0499241307030976E-4</v>
       </c>
     </row>
     <row r="5">
@@ -149,13 +150,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>4.066267089880354E-5</v>
+        <v>2.3104065255007958E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>9.63258290780013E-5</v>
+        <v>7.932316036944326E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.4073969916195432E-4</v>
+        <v>1.4180947105537703E-4</v>
       </c>
     </row>
     <row r="6">
@@ -163,13 +164,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>1.869387293371952E-5</v>
+        <v>8.646828111427647E-6</v>
       </c>
       <c r="C6" t="n">
-        <v>7.902830121400933E-5</v>
+        <v>6.644696867676565E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.295011353931652E-4</v>
+        <v>1.263252810724685E-4</v>
       </c>
     </row>
     <row r="7">
@@ -177,13 +178,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>2.373439503542935E-5</v>
+        <v>9.179547458171144E-6</v>
       </c>
       <c r="C7" t="n">
-        <v>8.079189053352592E-5</v>
+        <v>6.467854885561679E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>1.3057129400170965E-4</v>
+        <v>1.2415963629587934E-4</v>
       </c>
     </row>
     <row r="8">
@@ -191,13 +192,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.9125208487619842E-5</v>
+        <v>6.418305308349819E-6</v>
       </c>
       <c r="C8" t="n">
-        <v>7.424212812400549E-5</v>
+        <v>5.958575866947057E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>1.2258946885169815E-4</v>
+        <v>1.1609686222442757E-4</v>
       </c>
     </row>
     <row r="9">
@@ -205,13 +206,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.9731264210390855E-5</v>
+        <v>5.545550427173539E-6</v>
       </c>
       <c r="C9" t="n">
-        <v>7.056599148624484E-5</v>
+        <v>5.558974626214083E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>1.1634016242442423E-4</v>
+        <v>1.0869655299211765E-4</v>
       </c>
     </row>
     <row r="10">
@@ -219,13 +220,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.85267778039415E-5</v>
+        <v>4.525963453805099E-6</v>
       </c>
       <c r="C10" t="n">
-        <v>6.592130203227484E-5</v>
+        <v>5.156964002147228E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>1.0921448105452198E-4</v>
+        <v>1.0207440272727613E-4</v>
       </c>
     </row>
     <row r="11">
@@ -233,13 +234,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.7507169858825505E-5</v>
+        <v>3.7002837094798485E-6</v>
       </c>
       <c r="C11" t="n">
-        <v>6.179297058571939E-5</v>
+        <v>4.7775854971093796E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>1.0244479312415438E-4</v>
+        <v>9.707933683018867E-5</v>
       </c>
     </row>
     <row r="12">
@@ -247,13 +248,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.6237684542212513E-5</v>
+        <v>2.915025414602481E-6</v>
       </c>
       <c r="C12" t="n">
-        <v>5.766187732111343E-5</v>
+        <v>4.413517038586718E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>9.610309374018091E-5</v>
+        <v>9.234873125592463E-5</v>
       </c>
     </row>
   </sheetData>
@@ -302,13 +303,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.4234111911400329E-4</v>
+        <v>1.321309503571064E-4</v>
       </c>
       <c r="C3" t="n">
-        <v>1.7410737517854685E-4</v>
+        <v>1.5906024317168996E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.1177124659676262E-4</v>
+        <v>1.9915674766156862E-4</v>
       </c>
     </row>
     <row r="4">
@@ -316,13 +317,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>9.522312194822713E-5</v>
+        <v>7.869797045142158E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.412472388541856E-4</v>
+        <v>1.1798921860152201E-4</v>
       </c>
       <c r="D4" t="n">
-        <v>1.969848777966954E-4</v>
+        <v>1.6446646028906662E-4</v>
       </c>
     </row>
     <row r="5">
@@ -330,13 +331,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.3650663073306034E-4</v>
+        <v>1.1193768188714845E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>1.8264925733734033E-4</v>
+        <v>1.55034040041731E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>2.419131455878462E-4</v>
+        <v>2.072102533543733E-4</v>
       </c>
     </row>
     <row r="6">
@@ -344,13 +345,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>1.2206777110847239E-4</v>
+        <v>9.694215709366194E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.7121983881448392E-4</v>
+        <v>1.4128201624211473E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>2.3444985110901046E-4</v>
+        <v>1.9344802649252357E-4</v>
       </c>
     </row>
     <row r="7">
@@ -358,13 +359,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1.2106580584886212E-4</v>
+        <v>9.550556785940327E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.7059524707705733E-4</v>
+        <v>1.4067106102384533E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>2.3131185950273967E-4</v>
+        <v>1.9302546299259843E-4</v>
       </c>
     </row>
     <row r="8">
@@ -372,13 +373,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.1685664954001704E-4</v>
+        <v>9.165961391702541E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.6612517615724673E-4</v>
+        <v>1.3580939913077398E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>2.2616193458997375E-4</v>
+        <v>1.867350677754527E-4</v>
       </c>
     </row>
     <row r="9">
@@ -386,13 +387,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.129705263229843E-4</v>
+        <v>8.791019704620702E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>1.616111347609355E-4</v>
+        <v>1.3160267990867816E-4</v>
       </c>
       <c r="D9" t="n">
-        <v>2.205205149727174E-4</v>
+        <v>1.8040262382311708E-4</v>
       </c>
     </row>
     <row r="10">
@@ -400,13 +401,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.0835163047234861E-4</v>
+        <v>8.473049693727177E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.574281033005782E-4</v>
+        <v>1.275978521831733E-4</v>
       </c>
       <c r="D10" t="n">
-        <v>2.1514583265394506E-4</v>
+        <v>1.743737911306308E-4</v>
       </c>
     </row>
     <row r="11">
@@ -414,13 +415,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.0375552191583413E-4</v>
+        <v>8.133990686235358E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.5308354835585544E-4</v>
+        <v>1.2351688629964663E-4</v>
       </c>
       <c r="D11" t="n">
-        <v>2.0967349030815037E-4</v>
+        <v>1.6806743081053285E-4</v>
       </c>
     </row>
     <row r="12">
@@ -428,13 +429,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>9.937337345717014E-5</v>
+        <v>7.81739423510423E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.4891820576746042E-4</v>
+        <v>1.1963184664588768E-4</v>
       </c>
       <c r="D12" t="n">
-        <v>2.0509512774961585E-4</v>
+        <v>1.620636634430414E-4</v>
       </c>
     </row>
   </sheetData>
@@ -483,13 +484,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>7.091956719175574E-5</v>
+        <v>4.9787157851806024E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0012419555022948E-4</v>
+        <v>6.69696848441032E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.2561428553158117E-4</v>
+        <v>9.063494996778571E-5</v>
       </c>
     </row>
     <row r="4">
@@ -497,13 +498,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>1.792662214545147E-6</v>
+        <v>-1.3278283082400458E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>3.8852002550604517E-5</v>
+        <v>1.2106791515794812E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>6.312900859074564E-5</v>
+        <v>4.353175577339383E-5</v>
       </c>
     </row>
     <row r="5">
@@ -511,13 +512,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>3.157163141313998E-5</v>
+        <v>2.479548988842273E-6</v>
       </c>
       <c r="C5" t="n">
-        <v>7.01861784836642E-5</v>
+        <v>2.8080914880745678E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>9.909206573470313E-5</v>
+        <v>6.353878007119998E-5</v>
       </c>
     </row>
     <row r="6">
@@ -525,13 +526,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>1.1913185309001396E-5</v>
+        <v>-1.1082375396285412E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>5.448454658813061E-5</v>
+        <v>1.6944260680934262E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>8.434591013592258E-5</v>
+        <v>5.219329340367616E-5</v>
       </c>
     </row>
     <row r="7">
@@ -539,13 +540,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1.5331295270351175E-5</v>
+        <v>-1.0250838937366124E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>5.6572869540849805E-5</v>
+        <v>1.67071543521023E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>8.906056491634568E-5</v>
+        <v>5.1478551403650364E-5</v>
       </c>
     </row>
     <row r="8">
@@ -553,13 +554,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.2964943391336118E-5</v>
+        <v>-1.1809938309728926E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>5.334206251361747E-5</v>
+        <v>1.5120894477622793E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>8.50851456592981E-5</v>
+        <v>4.819183239361911E-5</v>
       </c>
     </row>
     <row r="9">
@@ -567,13 +568,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.2592341862762647E-5</v>
+        <v>-1.1433911460378286E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>5.1329178474598384E-5</v>
+        <v>1.3970156963247682E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>8.370360634499077E-5</v>
+        <v>4.561128354064777E-5</v>
       </c>
     </row>
     <row r="10">
@@ -581,13 +582,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.3111118162874652E-5</v>
+        <v>-1.1152570095221669E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>4.9429964331256216E-5</v>
+        <v>1.3211193959484722E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>8.20703852014122E-5</v>
+        <v>4.324621084105102E-5</v>
       </c>
     </row>
     <row r="11">
@@ -595,13 +596,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.3382851885801779E-5</v>
+        <v>-1.0788793758917434E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>4.743259322203999E-5</v>
+        <v>1.238568815910389E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>8.04132940392834E-5</v>
+        <v>4.0889281608799574E-5</v>
       </c>
     </row>
     <row r="12">
@@ -609,13 +610,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.3949066333960944E-5</v>
+        <v>-1.0377867502063745E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>4.559799473529613E-5</v>
+        <v>1.1677853931150583E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>7.869241474927907E-5</v>
+        <v>3.8711811167087584E-5</v>
       </c>
     </row>
   </sheetData>
@@ -664,13 +665,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.969098760068898E-4</v>
+        <v>-2.392895970023726E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>3.1040080826109673E-4</v>
+        <v>1.4297103881967275E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>4.315192800523705E-4</v>
+        <v>3.4971418084135783E-4</v>
       </c>
     </row>
     <row r="4">
@@ -678,13 +679,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.6759211590305301E-4</v>
+        <v>-4.1471948509341636E-4</v>
       </c>
       <c r="C4" t="n">
-        <v>7.420303133621358E-6</v>
+        <v>-1.7967897696135018E-4</v>
       </c>
       <c r="D4" t="n">
-        <v>1.6507023201189986E-4</v>
+        <v>9.496069543786287E-5</v>
       </c>
     </row>
     <row r="5">
@@ -692,13 +693,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-5.3959280704099406E-5</v>
+        <v>-2.930845326216788E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>1.2883429051932044E-4</v>
+        <v>-9.57155774715636E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>2.8510528571845553E-4</v>
+        <v>1.319373231923012E-4</v>
       </c>
     </row>
     <row r="6">
@@ -706,13 +707,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.2719508456997654E-4</v>
+        <v>-3.2122878217234307E-4</v>
       </c>
       <c r="C6" t="n">
-        <v>6.199148906617042E-5</v>
+        <v>-1.2795734139123505E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>2.2342113791467525E-4</v>
+        <v>1.0406390064731366E-4</v>
       </c>
     </row>
     <row r="7">
@@ -720,13 +721,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.1444371498336799E-4</v>
+        <v>-2.924082213219916E-4</v>
       </c>
       <c r="C7" t="n">
-        <v>7.028460193259142E-5</v>
+        <v>-1.1548939327923678E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>2.224994604050093E-4</v>
+        <v>9.535948356576185E-5</v>
       </c>
     </row>
     <row r="8">
@@ -734,13 +735,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.1602112608096509E-4</v>
+        <v>-2.698499590560676E-4</v>
       </c>
       <c r="C8" t="n">
-        <v>6.372057492355502E-5</v>
+        <v>-1.0277602196613199E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>2.070026719957699E-4</v>
+        <v>8.97575717319912E-5</v>
       </c>
     </row>
     <row r="9">
@@ -748,13 +749,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.156089323024522E-4</v>
+        <v>-2.51190796877397E-4</v>
       </c>
       <c r="C9" t="n">
-        <v>6.092031344722925E-5</v>
+        <v>-9.214660061009936E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>1.9526273857856314E-4</v>
+        <v>8.454638734724671E-5</v>
       </c>
     </row>
     <row r="10">
@@ -762,13 +763,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.0762585291145778E-4</v>
+        <v>-2.317559370958257E-4</v>
       </c>
       <c r="C10" t="n">
-        <v>5.983537837627215E-5</v>
+        <v>-8.033350075912207E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>1.880242741462638E-4</v>
+        <v>8.51911686734774E-5</v>
       </c>
     </row>
     <row r="11">
@@ -776,13 +777,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.0157002816310476E-4</v>
+        <v>-2.1491876251519484E-4</v>
       </c>
       <c r="C11" t="n">
-        <v>5.801942080597748E-5</v>
+        <v>-7.019336339437791E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>1.8345924067868203E-4</v>
+        <v>8.6972560817688E-5</v>
       </c>
     </row>
     <row r="12">
@@ -790,13 +791,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-9.51560195040485E-5</v>
+        <v>-1.9894384196889628E-4</v>
       </c>
       <c r="C12" t="n">
-        <v>5.678535102248881E-5</v>
+        <v>-6.062744978772601E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.7974423837349365E-4</v>
+        <v>9.05264354029736E-5</v>
       </c>
     </row>
   </sheetData>
@@ -845,13 +846,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>6.156585308675435E-5</v>
+        <v>1.95138463760515E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.4249870389588328E-4</v>
+        <v>1.0679922473323313E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.2916338951658227E-4</v>
+        <v>1.8266506837513993E-4</v>
       </c>
     </row>
     <row r="4">
@@ -859,13 +860,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-5.063005796825176E-5</v>
+        <v>-9.931005438529578E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>5.987462174207477E-5</v>
+        <v>2.4146970350405688E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.8054911335606014E-4</v>
+        <v>1.425832872633328E-4</v>
       </c>
     </row>
     <row r="5">
@@ -873,13 +874,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-2.2598096809953933E-5</v>
+        <v>-6.533051049515269E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>9.187242548310989E-5</v>
+        <v>5.591506834827563E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>2.0739160982521365E-4</v>
+        <v>1.8293807861086215E-4</v>
       </c>
     </row>
     <row r="6">
@@ -887,13 +888,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-3.7711965669774794E-5</v>
+        <v>-7.250428729137006E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>7.841866398592984E-5</v>
+        <v>4.274852145992803E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.985100849150418E-4</v>
+        <v>1.680369559692019E-4</v>
       </c>
     </row>
     <row r="7">
@@ -901,13 +902,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-3.715704133176009E-5</v>
+        <v>-7.0259787493344E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>7.623138381577491E-5</v>
+        <v>4.199345583400073E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>1.9921456305732884E-4</v>
+        <v>1.628776897958317E-4</v>
       </c>
     </row>
     <row r="8">
@@ -915,13 +916,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.512065212675169E-5</v>
+        <v>-6.38679027060347E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>7.482911173579641E-5</v>
+        <v>4.1447600582258796E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>1.9999305612982234E-4</v>
+        <v>1.5785186567998966E-4</v>
       </c>
     </row>
     <row r="9">
@@ -929,13 +930,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-3.270020690573896E-5</v>
+        <v>-5.913631009924375E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>7.321546035986447E-5</v>
+        <v>4.0932140508342795E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>2.003662498252907E-4</v>
+        <v>1.5340101904977972E-4</v>
       </c>
     </row>
     <row r="10">
@@ -943,13 +944,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-3.2670830090539705E-5</v>
+        <v>-5.426308239084516E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>7.218522024336013E-5</v>
+        <v>4.08888150681996E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>2.011900986651373E-4</v>
+        <v>1.5014775248632666E-4</v>
       </c>
     </row>
     <row r="11">
@@ -957,13 +958,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-3.1954274405012885E-5</v>
+        <v>-4.9666623019256114E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>7.104997308005188E-5</v>
+        <v>4.066449810960983E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>2.0120640228114231E-4</v>
+        <v>1.4854478871554634E-4</v>
       </c>
     </row>
     <row r="12">
@@ -971,13 +972,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-3.108729689855737E-5</v>
+        <v>-4.532674548028882E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>6.997309380519168E-5</v>
+        <v>4.047765961829808E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.9780087326843026E-4</v>
+        <v>1.4507371531150188E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1026,13 +1027,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>7.535549971350055E-5</v>
+        <v>8.721657628622889E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>9.861534681090082E-5</v>
+        <v>1.1752058467965007E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>1.333162508321451E-4</v>
+        <v>1.530537822997493E-4</v>
       </c>
     </row>
     <row r="4">
@@ -1040,13 +1041,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.7488798038263326E-5</v>
+        <v>7.816440911465805E-6</v>
       </c>
       <c r="C4" t="n">
-        <v>1.866169703499179E-5</v>
+        <v>4.770011639371209E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>6.808093575166314E-5</v>
+        <v>9.116857971945472E-5</v>
       </c>
     </row>
     <row r="5">
@@ -1054,13 +1055,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>2.145657360367816E-5</v>
+        <v>4.5720877449174526E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>5.810230049015097E-5</v>
+        <v>8.788655599913064E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.1672114879853291E-4</v>
+        <v>1.3570830285278984E-4</v>
       </c>
     </row>
     <row r="6">
@@ -1068,13 +1069,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-2.467571785470922E-7</v>
+        <v>2.579943242853E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>3.716966295057751E-5</v>
+        <v>6.767800109813021E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>9.241610800456484E-5</v>
+        <v>1.17334638391084E-4</v>
       </c>
     </row>
     <row r="7">
@@ -1082,13 +1083,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>4.5296057763760864E-6</v>
+        <v>2.861148757294027E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>3.942455132685802E-5</v>
+        <v>6.997105445277863E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>9.888715741288626E-5</v>
+        <v>1.2090407016321982E-4</v>
       </c>
     </row>
     <row r="8">
@@ -1096,13 +1097,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>2.4821459851797685E-6</v>
+        <v>2.5477005101286777E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>3.601156468420611E-5</v>
+        <v>6.508017389548949E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>9.297592787337224E-5</v>
+        <v>1.1561015011227249E-4</v>
       </c>
     </row>
     <row r="9">
@@ -1110,13 +1111,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>2.228919309847089E-6</v>
+        <v>2.390502241257878E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>3.4441502529932155E-5</v>
+        <v>6.254456496533622E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>9.035211712052628E-5</v>
+        <v>1.1261097602545511E-4</v>
       </c>
     </row>
     <row r="10">
@@ -1124,13 +1125,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>2.01364424962227E-6</v>
+        <v>2.2324453514970134E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>3.30062220558337E-5</v>
+        <v>5.9809801331028425E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>8.734314858580059E-5</v>
+        <v>1.0900848320432769E-4</v>
       </c>
     </row>
     <row r="11">
@@ -1138,13 +1139,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.5057095810933392E-6</v>
+        <v>2.0776454864763682E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>3.1523060502715715E-5</v>
+        <v>5.7162838467490845E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>8.427867423922235E-5</v>
+        <v>1.0560439096478648E-4</v>
       </c>
     </row>
     <row r="12">
@@ -1152,13 +1153,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>7.834444530083933E-7</v>
+        <v>1.914381288909815E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>3.0188605535160076E-5</v>
+        <v>5.466497577439216E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>8.161693190649118E-5</v>
+        <v>1.0226972833187942E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1207,13 +1208,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>3.838692521586176E-5</v>
+        <v>2.130875173104297E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>9.678035335468398E-5</v>
+        <v>6.583591952489932E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.525415025179542E-4</v>
+        <v>1.4921995401528528E-4</v>
       </c>
     </row>
     <row r="4">
@@ -1221,13 +1222,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-8.31819394785396E-5</v>
+        <v>-1.0583572545528926E-4</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.282309170464293E-5</v>
+        <v>-2.3132349031530753E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>6.659445156659765E-5</v>
+        <v>8.618927169777026E-5</v>
       </c>
     </row>
     <row r="5">
@@ -1235,13 +1236,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-4.0306215027923415E-5</v>
+        <v>-6.531572032048709E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>2.5242487551298982E-5</v>
+        <v>8.914716296415629E-6</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0782068020118904E-4</v>
+        <v>1.0599787893864002E-4</v>
       </c>
     </row>
     <row r="6">
@@ -1249,13 +1250,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-5.584641451055214E-5</v>
+        <v>-7.822137691295523E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>9.465957493670027E-6</v>
+        <v>-3.961791151852842E-6</v>
       </c>
       <c r="D6" t="n">
-        <v>8.785510861463078E-5</v>
+        <v>9.310910345751719E-5</v>
       </c>
     </row>
     <row r="7">
@@ -1263,13 +1264,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-5.791281469853503E-5</v>
+        <v>-7.954623015244926E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>6.890637466857658E-6</v>
+        <v>-4.915858281829588E-6</v>
       </c>
       <c r="D7" t="n">
-        <v>8.339609803451514E-5</v>
+        <v>9.017785200491133E-5</v>
       </c>
     </row>
     <row r="8">
@@ -1277,13 +1278,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-5.211914619890629E-5</v>
+        <v>-7.447965492048035E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>7.044785077397334E-6</v>
+        <v>-4.7270019677769645E-6</v>
       </c>
       <c r="D8" t="n">
-        <v>7.903685186175814E-5</v>
+        <v>8.610967487869588E-5</v>
       </c>
     </row>
     <row r="9">
@@ -1291,13 +1292,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-5.104715467030493E-5</v>
+        <v>-7.063365385141767E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>5.9422106199520025E-6</v>
+        <v>-5.097668725172298E-6</v>
       </c>
       <c r="D9" t="n">
-        <v>7.402615438427571E-5</v>
+        <v>8.217096730004764E-5</v>
       </c>
     </row>
     <row r="10">
@@ -1305,13 +1306,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-4.825407256183064E-5</v>
+        <v>-6.606512253188466E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>5.719284539600355E-6</v>
+        <v>-4.874123055601195E-6</v>
       </c>
       <c r="D10" t="n">
-        <v>7.015946324139695E-5</v>
+        <v>7.877620573903604E-5</v>
       </c>
     </row>
     <row r="11">
@@ -1319,13 +1320,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-4.698767255949897E-5</v>
+        <v>-6.203808279064571E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>5.2554716778030546E-6</v>
+        <v>-4.8879781028387E-6</v>
       </c>
       <c r="D11" t="n">
-        <v>6.730848621077288E-5</v>
+        <v>7.517835188642285E-5</v>
       </c>
     </row>
     <row r="12">
@@ -1333,13 +1334,194 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-4.703323605674094E-5</v>
+        <v>-5.871624686083546E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>4.8286052348918824E-6</v>
+        <v>-4.8758048240662885E-6</v>
       </c>
       <c r="D12" t="n">
-        <v>6.469626712373302E-5</v>
+        <v>7.179410435348385E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0488331525601943</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.059861259112784934</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.07017884960667811</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.038560839201852</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.052649922494949875</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.06813902576516045</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.04458729208784201</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.059780378427867965</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.07629575310627734</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.041967620800412574</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0581313020118302</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.07482967802935513</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.04071314829069662</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.05698695601723878</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.07339283921723734</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.039080315338782985</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.055419639645270774</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.07115203587814051</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.03733895996181756</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.05363635755381336</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.06848708607852265</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.035713833422873056</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.05192031405262249</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0659106717818926</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.03409582370036506</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0502063660010609</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.06370831419320314</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.03255581261243484</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.04854434183038276</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.06142782997575623</v>
       </c>
     </row>
   </sheetData>
@@ -1388,13 +1570,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.335307136246534E-4</v>
+        <v>2.1466379867001974E-4</v>
       </c>
       <c r="C3" t="n">
-        <v>2.1421058772919037E-4</v>
+        <v>2.854393286107382E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.844585185242225E-4</v>
+        <v>3.640036849286925E-4</v>
       </c>
     </row>
     <row r="4">
@@ -1402,13 +1584,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>2.289553886926821E-5</v>
+        <v>3.8082540235263085E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.1417334721353804E-4</v>
+        <v>1.2890820972941638E-4</v>
       </c>
       <c r="D4" t="n">
-        <v>2.1888979214301562E-4</v>
+        <v>2.1714795364491035E-4</v>
       </c>
     </row>
     <row r="5">
@@ -1416,13 +1598,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>9.125734908659531E-5</v>
+        <v>1.2996912435568554E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>1.980479211853999E-4</v>
+        <v>2.213750629365622E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>3.058176986274442E-4</v>
+        <v>3.288728282121974E-4</v>
       </c>
     </row>
     <row r="6">
@@ -1430,13 +1612,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>5.238699255762715E-5</v>
+        <v>7.667859297772915E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.6154929623911528E-4</v>
+        <v>1.718507015771847E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>2.741024439708347E-4</v>
+        <v>2.7059912315538975E-4</v>
       </c>
     </row>
     <row r="7">
@@ -1444,13 +1626,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>5.6024522250209954E-5</v>
+        <v>8.365749970892108E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.653221013189827E-4</v>
+        <v>1.7749856631138426E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>2.744419918628091E-4</v>
+        <v>2.787706024802605E-4</v>
       </c>
     </row>
     <row r="8">
@@ -1458,13 +1640,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>4.751849075254111E-5</v>
+        <v>7.329368529229549E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.5626373036631993E-4</v>
+        <v>1.637545759456649E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>2.662794804141646E-4</v>
+        <v>2.5676100096258905E-4</v>
       </c>
     </row>
     <row r="9">
@@ -1472,13 +1654,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>4.253126594277566E-5</v>
+        <v>7.007752077568598E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>1.5097011487039203E-4</v>
+        <v>1.5697473736541503E-4</v>
       </c>
       <c r="D9" t="n">
-        <v>2.649044294095296E-4</v>
+        <v>2.469983573844946E-4</v>
       </c>
     </row>
     <row r="10">
@@ -1486,13 +1668,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>3.71850484046345E-5</v>
+        <v>6.60964215769977E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.4563419410385648E-4</v>
+        <v>1.4896985511581184E-4</v>
       </c>
       <c r="D10" t="n">
-        <v>2.609988641447206E-4</v>
+        <v>2.3432636019043104E-4</v>
       </c>
     </row>
     <row r="11">
@@ -1500,13 +1682,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>3.3764248122052625E-5</v>
+        <v>6.0889228290935715E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.4036986394629382E-4</v>
+        <v>1.4162178040273116E-4</v>
       </c>
       <c r="D11" t="n">
-        <v>2.5523590006742763E-4</v>
+        <v>2.2324797850806563E-4</v>
       </c>
     </row>
     <row r="12">
@@ -1514,13 +1696,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>3.194649872422631E-5</v>
+        <v>5.625652069363385E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.3539043966379825E-4</v>
+        <v>1.345450743227435E-4</v>
       </c>
       <c r="D12" t="n">
-        <v>2.49681084726227E-4</v>
+        <v>2.126615685217408E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1569,13 +1751,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.1137362039218465E-4</v>
+        <v>8.22013076664712E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.5449860641343461E-4</v>
+        <v>1.29330904049136E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>1.8786138045485154E-4</v>
+        <v>1.5973350473931025E-4</v>
       </c>
     </row>
     <row r="4">
@@ -1583,13 +1765,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>4.671565685417173E-5</v>
+        <v>1.8234188510435704E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>9.66822093617025E-5</v>
+        <v>7.85109753270316E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.430004876476057E-4</v>
+        <v>1.277975009320403E-4</v>
       </c>
     </row>
     <row r="5">
@@ -1597,13 +1779,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0079001276719632E-4</v>
+        <v>5.321011721869254E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>1.566536826326961E-4</v>
+        <v>1.2268762989244125E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>2.1162633016370063E-4</v>
+        <v>1.8030193818217573E-4</v>
       </c>
     </row>
     <row r="6">
@@ -1611,13 +1793,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>7.551188988151971E-5</v>
+        <v>3.3017522770577504E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.347013308362997E-4</v>
+        <v>1.040089825084729E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>1.9694698732431023E-4</v>
+        <v>1.6534942957003508E-4</v>
       </c>
     </row>
     <row r="7">
@@ -1625,13 +1807,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>8.249116413677101E-5</v>
+        <v>3.792071253917907E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.4313213403187625E-4</v>
+        <v>1.0781250918023486E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>2.083397808266039E-4</v>
+        <v>1.6883435236621832E-4</v>
       </c>
     </row>
     <row r="8">
@@ -1639,13 +1821,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>7.571999936887875E-5</v>
+        <v>3.4077311130970074E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.3599317866687944E-4</v>
+        <v>1.0198143093451393E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>2.0283924506731474E-4</v>
+        <v>1.6098506171926283E-4</v>
       </c>
     </row>
     <row r="9">
@@ -1653,13 +1835,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>7.379342181082862E-5</v>
+        <v>3.418997761418789E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>1.3377291955823535E-4</v>
+        <v>9.920108088129111E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>2.0071618873763677E-4</v>
+        <v>1.556320251262437E-4</v>
       </c>
     </row>
     <row r="10">
@@ -1667,13 +1849,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>6.942584441576926E-5</v>
+        <v>3.3277363312934106E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.292942323036604E-4</v>
+        <v>9.553732283391341E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>1.9578611562174242E-4</v>
+        <v>1.4899593982381124E-4</v>
       </c>
     </row>
     <row r="11">
@@ -1681,13 +1863,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>6.616755565218087E-5</v>
+        <v>3.2774084300804064E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.254611136238122E-4</v>
+        <v>9.214042824855716E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>1.8882980663187358E-4</v>
+        <v>1.4269805637921707E-4</v>
       </c>
     </row>
     <row r="12">
@@ -1695,13 +1877,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>6.259302901195082E-5</v>
+        <v>3.133357408665693E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.2137822540814068E-4</v>
+        <v>8.878794293686127E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.818780111076027E-4</v>
+        <v>1.3728771859716142E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1750,13 +1932,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>3.489487169049455E-5</v>
+        <v>2.5255912370346104E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>4.883943272570913E-5</v>
+        <v>4.5653253823767565E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>6.981910487149082E-5</v>
+        <v>6.615423603837265E-5</v>
       </c>
     </row>
     <row r="4">
@@ -1764,13 +1946,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.8904128028199486E-5</v>
+        <v>-2.5427881535440465E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.489106480457413E-6</v>
+        <v>-5.233086979062421E-6</v>
       </c>
       <c r="D4" t="n">
-        <v>3.682751197053154E-5</v>
+        <v>2.2111537435875617E-5</v>
       </c>
     </row>
     <row r="5">
@@ -1778,13 +1960,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.1473513753769705E-6</v>
+        <v>-3.994754688667782E-6</v>
       </c>
       <c r="C5" t="n">
-        <v>2.3450990313058582E-5</v>
+        <v>1.5847707723970122E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>5.7890060207493196E-5</v>
+        <v>4.481769168351729E-5</v>
       </c>
     </row>
     <row r="6">
@@ -1792,13 +1974,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.2373878199038512E-5</v>
+        <v>-1.8162264024810092E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>9.720877136062259E-6</v>
+        <v>2.3774775695516916E-6</v>
       </c>
       <c r="D6" t="n">
-        <v>4.680769206206456E-5</v>
+        <v>3.1564260841055784E-5</v>
       </c>
     </row>
     <row r="7">
@@ -1806,13 +1988,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.1509070506952588E-5</v>
+        <v>-1.6424443772511862E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.134680468473094E-5</v>
+        <v>4.1497825466715375E-6</v>
       </c>
       <c r="D7" t="n">
-        <v>4.7780265277822834E-5</v>
+        <v>3.5288613269586296E-5</v>
       </c>
     </row>
     <row r="8">
@@ -1820,13 +2002,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.2956950294621884E-5</v>
+        <v>-1.686315263373901E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>9.02855656706701E-6</v>
+        <v>2.154800312509985E-6</v>
       </c>
       <c r="D8" t="n">
-        <v>4.3718334317359946E-5</v>
+        <v>3.267566041802921E-5</v>
       </c>
     </row>
     <row r="9">
@@ -1834,13 +2016,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.3169256736164048E-5</v>
+        <v>-1.6791328023704027E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>8.321261606812771E-6</v>
+        <v>1.6936501733271902E-6</v>
       </c>
       <c r="D9" t="n">
-        <v>4.1771352586950715E-5</v>
+        <v>3.08299060084788E-5</v>
       </c>
     </row>
     <row r="10">
@@ -1848,13 +2030,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.2929271046744237E-5</v>
+        <v>-1.6389744268510475E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>7.540860428944782E-6</v>
+        <v>1.2002563650570646E-6</v>
       </c>
       <c r="D10" t="n">
-        <v>3.9092386977104736E-5</v>
+        <v>2.8907030791939836E-5</v>
       </c>
     </row>
     <row r="11">
@@ -1862,13 +2044,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.277442495983109E-5</v>
+        <v>-1.6153497570374754E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>6.8449970226986405E-6</v>
+        <v>7.307615613229383E-7</v>
       </c>
       <c r="D11" t="n">
-        <v>3.678654261968376E-5</v>
+        <v>2.7025136922601732E-5</v>
       </c>
     </row>
     <row r="12">
@@ -1876,13 +2058,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.3127693339336812E-5</v>
+        <v>-1.5822399421715644E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>6.191210801842718E-6</v>
+        <v>3.200620727272455E-7</v>
       </c>
       <c r="D12" t="n">
-        <v>3.4456108138368896E-5</v>
+        <v>2.5269233320036632E-5</v>
       </c>
     </row>
   </sheetData>
@@ -1931,13 +2113,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>5.269054748315756E-5</v>
+        <v>4.564189377217571E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>6.952223378832964E-5</v>
+        <v>6.0505385971905015E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>8.012816312414841E-5</v>
+        <v>7.476185254900864E-5</v>
       </c>
     </row>
     <row r="4">
@@ -1945,13 +2127,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>2.0409756307212845E-5</v>
+        <v>2.2227252773871332E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>3.9065230223776586E-5</v>
+        <v>4.2734401901601234E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>5.363519431852723E-5</v>
+        <v>6.76926754431112E-5</v>
       </c>
     </row>
     <row r="5">
@@ -1959,13 +2141,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>3.379424696262023E-5</v>
+        <v>3.208889043472125E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>5.3163984385203124E-5</v>
+        <v>5.375502964814054E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>6.944679175742462E-5</v>
+        <v>7.855890970803236E-5</v>
       </c>
     </row>
     <row r="6">
@@ -1973,13 +2155,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>2.5488092997502298E-5</v>
+        <v>2.688801747815481E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>4.645994305067936E-5</v>
+        <v>4.923335325006838E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>6.233514861660944E-5</v>
+        <v>7.622582473011991E-5</v>
       </c>
     </row>
     <row r="7">
@@ -1987,13 +2169,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>2.5273298902273348E-5</v>
+        <v>2.559791286191849E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>4.594788002151691E-5</v>
+        <v>4.828761507084192E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>6.135032985259328E-5</v>
+        <v>7.512374124621325E-5</v>
       </c>
     </row>
     <row r="8">
@@ -2001,13 +2183,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>2.348241034069262E-5</v>
+        <v>2.426984198464637E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>4.354633651957676E-5</v>
+        <v>4.596816561603149E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>5.837684674111875E-5</v>
+        <v>7.228304900396426E-5</v>
       </c>
     </row>
     <row r="9">
@@ -2015,13 +2197,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>2.196590053049339E-5</v>
+        <v>2.2771214336831208E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>4.153565681913716E-5</v>
+        <v>4.374334249401815E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>5.639685531721535E-5</v>
+        <v>6.933496728707764E-5</v>
       </c>
     </row>
     <row r="10">
@@ -2029,13 +2211,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>2.001190627514488E-5</v>
+        <v>2.1597616403998034E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>3.951683236068289E-5</v>
+        <v>4.157919800662963E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>5.4412698163066124E-5</v>
+        <v>6.629794391618432E-5</v>
       </c>
     </row>
     <row r="11">
@@ -2043,13 +2225,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.809150982015601E-5</v>
+        <v>2.0422536553199466E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>3.7605222186242396E-5</v>
+        <v>3.946547521109159E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>5.247148935653469E-5</v>
+        <v>6.331282483813652E-5</v>
       </c>
     </row>
     <row r="12">
@@ -2057,13 +2239,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.6307322147875455E-5</v>
+        <v>1.933228698205365E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>3.576521158314071E-5</v>
+        <v>3.745689333924117E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>5.0857186905554935E-5</v>
+        <v>6.0430584571639565E-5</v>
       </c>
     </row>
   </sheetData>
@@ -2112,13 +2294,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>5.63424467209158E-5</v>
+        <v>3.6457096745814566E-6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.3126379639707031E-4</v>
+        <v>8.258124115205689E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>2.4864761166944356E-4</v>
+        <v>1.610780257286061E-4</v>
       </c>
     </row>
     <row r="4">
@@ -2126,13 +2308,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.073650809015569E-4</v>
+        <v>-1.3254369803644255E-4</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.941707487155559E-6</v>
+        <v>-1.9130568042268566E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.2862408141500048E-4</v>
+        <v>6.0006138802124296E-5</v>
       </c>
     </row>
     <row r="5">
@@ -2140,13 +2322,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-6.694295579916548E-5</v>
+        <v>-1.0070696758098737E-4</v>
       </c>
       <c r="C5" t="n">
-        <v>3.606743655753299E-5</v>
+        <v>1.608727917941119E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>1.5779282512212064E-4</v>
+        <v>1.086018661391303E-4</v>
       </c>
     </row>
     <row r="6">
@@ -2154,13 +2336,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-8.353218410716925E-5</v>
+        <v>-1.1644167053502133E-4</v>
       </c>
       <c r="C6" t="n">
-        <v>1.873630681574646E-5</v>
+        <v>1.685964277938421E-6</v>
       </c>
       <c r="D6" t="n">
-        <v>1.4029671056178664E-4</v>
+        <v>8.457235069407095E-5</v>
       </c>
     </row>
     <row r="7">
@@ -2168,13 +2350,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-8.93664786589838E-5</v>
+        <v>-1.1307114843839389E-4</v>
       </c>
       <c r="C7" t="n">
-        <v>1.5003014982292908E-5</v>
+        <v>2.1346763199308912E-7</v>
       </c>
       <c r="D7" t="n">
-        <v>1.3472066024396062E-4</v>
+        <v>7.594876550194899E-5</v>
       </c>
     </row>
     <row r="8">
@@ -2182,13 +2364,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.320937175227101E-5</v>
+        <v>-1.0714746093762467E-4</v>
       </c>
       <c r="C8" t="n">
-        <v>1.530016811253724E-5</v>
+        <v>4.6338890534742456E-7</v>
       </c>
       <c r="D8" t="n">
-        <v>1.3337341997235756E-4</v>
+        <v>7.158904479596954E-5</v>
       </c>
     </row>
     <row r="9">
@@ -2196,13 +2378,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-8.239276748975726E-5</v>
+        <v>-1.0196089418506747E-4</v>
       </c>
       <c r="C9" t="n">
-        <v>1.4125470081844684E-5</v>
+        <v>1.8659189301447017E-7</v>
       </c>
       <c r="D9" t="n">
-        <v>1.3059036585160366E-4</v>
+        <v>6.714337987806835E-5</v>
       </c>
     </row>
     <row r="10">
@@ -2210,13 +2392,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-7.994794492147367E-5</v>
+        <v>-9.661959831055222E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.3951378422584053E-5</v>
+        <v>5.537108046011506E-7</v>
       </c>
       <c r="D10" t="n">
-        <v>1.2977542033775651E-4</v>
+        <v>6.351990355543257E-5</v>
       </c>
     </row>
     <row r="11">
@@ -2224,13 +2406,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-7.82788502438476E-5</v>
+        <v>-9.182012363836234E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.35057719453106E-5</v>
+        <v>6.532137280261538E-7</v>
       </c>
       <c r="D11" t="n">
-        <v>1.2481534878488207E-4</v>
+        <v>6.029423295910385E-5</v>
       </c>
     </row>
     <row r="12">
@@ -2238,13 +2420,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-7.97979504993474E-5</v>
+        <v>-8.722886366727717E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.3092230423868499E-5</v>
+        <v>7.703789814028644E-7</v>
       </c>
       <c r="D12" t="n">
-        <v>1.1901522500840828E-4</v>
+        <v>5.881487935858312E-5</v>
       </c>
     </row>
   </sheetData>
@@ -2293,13 +2475,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>9.758594159660214E-6</v>
+        <v>7.348806214160094E-6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.561677879826541E-5</v>
+        <v>1.3084228908537576E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>2.249558898358798E-5</v>
+        <v>1.89979655505295E-5</v>
       </c>
     </row>
     <row r="4">
@@ -2307,13 +2489,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.535009203447866E-6</v>
+        <v>-2.492806276616318E-6</v>
       </c>
       <c r="C4" t="n">
-        <v>6.952768369448205E-6</v>
+        <v>5.656615113245576E-6</v>
       </c>
       <c r="D4" t="n">
-        <v>1.4720110032071848E-5</v>
+        <v>1.252115083389477E-5</v>
       </c>
     </row>
     <row r="5">
@@ -2321,13 +2503,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.920307593022782E-6</v>
+        <v>1.772429202430625E-7</v>
       </c>
       <c r="C5" t="n">
-        <v>1.2643282893722446E-5</v>
+        <v>9.948302824062642E-6</v>
       </c>
       <c r="D5" t="n">
-        <v>2.1580758607290077E-5</v>
+        <v>1.7472797422529628E-5</v>
       </c>
     </row>
     <row r="6">
@@ -2335,13 +2517,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.2844206807816312E-6</v>
+        <v>-2.0515815386649875E-6</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0135991637107659E-5</v>
+        <v>7.851652188092424E-6</v>
       </c>
       <c r="D6" t="n">
-        <v>1.9335392193226395E-5</v>
+        <v>1.57811665518135E-5</v>
       </c>
     </row>
     <row r="7">
@@ -2349,13 +2531,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-9.828743952145076E-7</v>
+        <v>-1.8597319390888695E-6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0725411401855623E-5</v>
+        <v>8.243215819294555E-6</v>
       </c>
       <c r="D7" t="n">
-        <v>1.9996429326080102E-5</v>
+        <v>1.6043993385511926E-5</v>
       </c>
     </row>
     <row r="8">
@@ -2363,13 +2545,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.2961431786575484E-6</v>
+        <v>-2.2931393633656005E-6</v>
       </c>
       <c r="C8" t="n">
-        <v>1.011064874440811E-5</v>
+        <v>7.711207612471595E-6</v>
       </c>
       <c r="D8" t="n">
-        <v>1.89165930447901E-5</v>
+        <v>1.538357931584144E-5</v>
       </c>
     </row>
     <row r="9">
@@ -2377,13 +2559,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.35527628919838E-6</v>
+        <v>-2.3278891261890534E-6</v>
       </c>
       <c r="C9" t="n">
-        <v>9.844934414624075E-6</v>
+        <v>7.473447994983167E-6</v>
       </c>
       <c r="D9" t="n">
-        <v>1.822110769462304E-5</v>
+        <v>1.4884333297305689E-5</v>
       </c>
     </row>
     <row r="10">
@@ -2391,13 +2573,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.3742373114696646E-6</v>
+        <v>-2.44358590944075E-6</v>
       </c>
       <c r="C10" t="n">
-        <v>9.492663168732812E-6</v>
+        <v>7.168130477911577E-6</v>
       </c>
       <c r="D10" t="n">
-        <v>1.7380685351820214E-5</v>
+        <v>1.4304987196321651E-5</v>
       </c>
     </row>
     <row r="11">
@@ -2405,13 +2587,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.2291635700988022E-6</v>
+        <v>-2.5376806306094395E-6</v>
       </c>
       <c r="C11" t="n">
-        <v>9.159550941514867E-6</v>
+        <v>6.884452598448699E-6</v>
       </c>
       <c r="D11" t="n">
-        <v>1.6826793854481613E-5</v>
+        <v>1.3768032606068904E-5</v>
       </c>
     </row>
     <row r="12">
@@ -2419,13 +2601,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.025752771203109E-6</v>
+        <v>-2.6277948076199082E-6</v>
       </c>
       <c r="C12" t="n">
-        <v>8.833473931980752E-6</v>
+        <v>6.60664484311765E-6</v>
       </c>
       <c r="D12" t="n">
-        <v>1.6723043077294172E-5</v>
+        <v>1.3312566459599707E-5</v>
       </c>
     </row>
   </sheetData>
@@ -2474,13 +2656,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.5851425708668273E-5</v>
+        <v>-1.9298207376839703E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>2.62416236558564E-5</v>
+        <v>1.4362678153756038E-5</v>
       </c>
       <c r="D3" t="n">
-        <v>5.8210015966298155E-5</v>
+        <v>5.2568536871676024E-5</v>
       </c>
     </row>
     <row r="4">
@@ -2488,13 +2670,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-9.0275467436097E-5</v>
+        <v>-9.34583682116387E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.239677056370197E-5</v>
+        <v>-4.70179577623042E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0967562278109024E-5</v>
+        <v>4.024829351093553E-6</v>
       </c>
     </row>
     <row r="5">
@@ -2502,13 +2684,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-6.93738690568466E-5</v>
+        <v>-7.063924343957816E-5</v>
       </c>
       <c r="C5" t="n">
-        <v>-7.762046962751636E-6</v>
+        <v>-2.3474510085199508E-5</v>
       </c>
       <c r="D5" t="n">
-        <v>4.415275828684073E-5</v>
+        <v>3.18741990933199E-5</v>
       </c>
     </row>
     <row r="6">
@@ -2516,13 +2698,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-8.791166913437717E-5</v>
+        <v>-9.001312089715171E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.4886187860625285E-5</v>
+        <v>-4.0434887547148955E-5</v>
       </c>
       <c r="D6" t="n">
-        <v>2.4824604907010056E-5</v>
+        <v>1.476284820927773E-5</v>
       </c>
     </row>
     <row r="7">
@@ -2530,13 +2712,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-8.56953704957714E-5</v>
+        <v>-8.657691529676711E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.353551924099664E-5</v>
+        <v>-3.828492171253377E-5</v>
       </c>
       <c r="D7" t="n">
-        <v>2.827269529738472E-5</v>
+        <v>1.8057938611361143E-5</v>
       </c>
     </row>
     <row r="8">
@@ -2544,13 +2726,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.543000172188495E-5</v>
+        <v>-8.717259973350987E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.5571396824989053E-5</v>
+        <v>-4.011235097376596E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>2.4460075765390306E-5</v>
+        <v>1.3931447290754947E-5</v>
       </c>
     </row>
     <row r="9">
@@ -2558,13 +2740,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-8.333013909066266E-5</v>
+        <v>-8.476622003803695E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>-2.59036917145582E-5</v>
+        <v>-3.9821876576417894E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>2.384227523147164E-5</v>
+        <v>1.3235005133571109E-5</v>
       </c>
     </row>
     <row r="10">
@@ -2572,13 +2754,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-8.105853336010979E-5</v>
+        <v>-8.315574256393687E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.6042816682326928E-5</v>
+        <v>-3.9580717285244625E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>2.2993964099507694E-5</v>
+        <v>1.2083697575724758E-5</v>
       </c>
     </row>
     <row r="11">
@@ -2586,13 +2768,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-7.949995843690645E-5</v>
+        <v>-8.17699724920845E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.6209378306993627E-5</v>
+        <v>-3.933623642556548E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>2.2265258954316328E-5</v>
+        <v>1.1806711698054251E-5</v>
       </c>
     </row>
     <row r="12">
@@ -2600,13 +2782,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-7.796808846250977E-5</v>
+        <v>-8.031313390342446E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.629121594501653E-5</v>
+        <v>-3.9045970715376377E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>2.165438549270456E-5</v>
+        <v>1.1534491491922419E-5</v>
       </c>
     </row>
   </sheetData>
@@ -2655,13 +2837,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>8.735369985747219E-5</v>
+        <v>4.8894196150823275E-5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.9511602990673083E-4</v>
+        <v>1.3866802146405102E-4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.9138353750147067E-4</v>
+        <v>2.5097515462131826E-4</v>
       </c>
     </row>
     <row r="4">
@@ -2669,13 +2851,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>-6.769407593302612E-5</v>
+        <v>-4.512384126738371E-5</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0617573158201675E-4</v>
+        <v>9.301648580140356E-5</v>
       </c>
       <c r="D4" t="n">
-        <v>2.798662649768939E-4</v>
+        <v>2.3324514076852545E-4</v>
       </c>
     </row>
     <row r="5">
@@ -2683,13 +2865,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>-7.121590034908226E-7</v>
+        <v>-1.225900961708885E-6</v>
       </c>
       <c r="C5" t="n">
-        <v>1.7864564318151508E-4</v>
+        <v>1.4223000635085352E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>3.6252691695435116E-4</v>
+        <v>2.866443949375089E-4</v>
       </c>
     </row>
     <row r="6">
@@ -2697,13 +2879,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>-3.6675062116670996E-5</v>
+        <v>-2.027441064989002E-5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.4867729185341546E-4</v>
+        <v>1.2092325672317414E-4</v>
       </c>
       <c r="D6" t="n">
-        <v>3.2602884925528113E-4</v>
+        <v>2.6235494189336865E-4</v>
       </c>
     </row>
     <row r="7">
@@ -2711,13 +2893,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>-3.6260989054248246E-5</v>
+        <v>-1.7347281733541507E-5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.4231967605716068E-4</v>
+        <v>1.1443191245358098E-4</v>
       </c>
       <c r="D7" t="n">
-        <v>3.13895613781596E-4</v>
+        <v>2.443433411084746E-4</v>
       </c>
     </row>
     <row r="8">
@@ -2725,13 +2907,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.8383307532960105E-5</v>
+        <v>-2.107367135840152E-5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.3329508253946126E-4</v>
+        <v>1.061889353436273E-4</v>
       </c>
       <c r="D8" t="n">
-        <v>2.942746275517486E-4</v>
+        <v>2.259787683667926E-4</v>
       </c>
     </row>
     <row r="9">
@@ -2739,13 +2921,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>-4.1487674686389105E-5</v>
+        <v>-2.3588017106031413E-5</v>
       </c>
       <c r="C9" t="n">
-        <v>1.237562814258342E-4</v>
+        <v>9.836013604337666E-5</v>
       </c>
       <c r="D9" t="n">
-        <v>2.7738348945265394E-4</v>
+        <v>2.1312228595179645E-4</v>
       </c>
     </row>
     <row r="10">
@@ -2753,13 +2935,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>-4.1871326422875945E-5</v>
+        <v>-2.544686784583761E-5</v>
       </c>
       <c r="C10" t="n">
-        <v>1.1624825461904845E-4</v>
+        <v>9.171975461299376E-5</v>
       </c>
       <c r="D10" t="n">
-        <v>2.615467945811246E-4</v>
+        <v>2.0486404521824456E-4</v>
       </c>
     </row>
     <row r="11">
@@ -2767,13 +2949,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>-4.430284656436626E-5</v>
+        <v>-2.79851277409775E-5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0844502477399524E-4</v>
+        <v>8.500612079534273E-5</v>
       </c>
       <c r="D11" t="n">
-        <v>2.473140329074424E-4</v>
+        <v>1.9424521414185432E-4</v>
       </c>
     </row>
     <row r="12">
@@ -2781,13 +2963,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>-4.672290288110072E-5</v>
+        <v>-3.098083824182788E-5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0120122210850753E-4</v>
+        <v>7.869517270453408E-5</v>
       </c>
       <c r="D12" t="n">
-        <v>2.3686679356430535E-4</v>
+        <v>1.8653621516662603E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>